<commit_message>
SFS with new tables
</commit_message>
<xml_diff>
--- a/hivwholeseq/tables/HIV_reservoir_all.xlsx
+++ b/hivwholeseq/tables/HIV_reservoir_all.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="357">
   <si>
     <t>id</t>
   </si>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t>N5-S2</t>
+  </si>
+  <si>
+    <t>PROBABLY 5b</t>
   </si>
   <si>
     <t>VK04-3106_PCR1</t>
@@ -1572,11 +1575,11 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1 2" xfId="22" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1 2" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="24" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1650,7 +1653,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="1" sqref="C76:C77 H13"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1727,6 +1730,7 @@
         <v>37530</v>
       </c>
       <c r="G3" s="7"/>
+      <c r="H3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
@@ -1766,6 +1770,7 @@
         <v>36878</v>
       </c>
       <c r="G5" s="7"/>
+      <c r="H5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
@@ -1784,6 +1789,7 @@
         <v>37700</v>
       </c>
       <c r="G6" s="7"/>
+      <c r="H6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
@@ -1939,7 +1945,7 @@
   <dimension ref="A1:F464"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="C76:C77 A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -8752,7 +8758,7 @@
   <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A58" activeCellId="1" sqref="C76:C77 A58"/>
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10752,8 +10758,8 @@
   </sheetPr>
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C77" activeCellId="0" sqref="C76:C77"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B31" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J49" activeCellId="0" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -11995,7 +12001,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>153</v>
@@ -12007,10 +12013,13 @@
         <v>154</v>
       </c>
       <c r="I49" s="0"/>
+      <c r="J49" s="0" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B50" s="10" t="str">
         <f aca="false">LEFT(A50, FIND("_", A50, 1) - 1)</f>
@@ -12022,22 +12031,25 @@
         <v>1</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>153</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H50" s="10" t="s">
         <v>154</v>
       </c>
       <c r="I50" s="0"/>
+      <c r="J50" s="0" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B51" s="10" t="str">
         <f aca="false">LEFT(A51, FIND("_", A51, 1) - 1)</f>
@@ -12055,7 +12067,7 @@
         <v>153</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H51" s="10" t="s">
         <v>149</v>
@@ -12064,7 +12076,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B52" s="10" t="str">
         <f aca="false">LEFT(A52, FIND("_", A52, 1) - 1)</f>
@@ -12091,20 +12103,20 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B53" s="0"/>
       <c r="C53" s="0"/>
       <c r="D53" s="0"/>
       <c r="E53" s="0"/>
       <c r="F53" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G53" s="10" t="s">
         <v>145</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I53" s="10" t="s">
         <v>147</v>
@@ -12112,14 +12124,14 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B54" s="10" t="str">
         <f aca="false">LEFT(A54, FIND("_", A54, 1) - 1)</f>
         <v>VK01-2965</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D54" s="10" t="n">
         <v>2</v>
@@ -12128,7 +12140,7 @@
         <v>79</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>88</v>
@@ -12140,14 +12152,14 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B55" s="10" t="str">
         <f aca="false">LEFT(A55, FIND("_", A55, 1) - 1)</f>
         <v>05HR-0269</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D55" s="10" t="n">
         <v>2</v>
@@ -12156,7 +12168,7 @@
         <v>79</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G55" s="10" t="s">
         <v>90</v>
@@ -12168,14 +12180,14 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B56" s="10" t="str">
         <f aca="false">LEFT(A56, FIND("_", A56, 1) - 1)</f>
         <v>VK09-1685</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D56" s="10" t="n">
         <v>2</v>
@@ -12184,7 +12196,7 @@
         <v>79</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>99</v>
@@ -12196,7 +12208,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B57" s="10" t="str">
         <f aca="false">LEFT(A57, FIND("_", A57, 1) - 1)</f>
@@ -12211,19 +12223,19 @@
         <v>79</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>102</v>
       </c>
       <c r="H57" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="10" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B58" s="10" t="str">
         <f aca="false">LEFT(A58, FIND("_", A58, 1) - 1)</f>
@@ -12238,19 +12250,19 @@
         <v>79</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B59" s="10" t="str">
         <f aca="false">LEFT(A59, FIND("_", A59, 1) - 1)</f>
@@ -12265,19 +12277,19 @@
         <v>79</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H59" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B60" s="10" t="str">
         <f aca="false">LEFT(A60, FIND("_", A60, 1) - 1)</f>
@@ -12292,19 +12304,19 @@
         <v>79</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G60" s="10" t="s">
         <v>129</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B61" s="10" t="str">
         <f aca="false">LEFT(A61, FIND("_", A61, 1) - 1)</f>
@@ -12319,19 +12331,19 @@
         <v>79</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>157</v>
       </c>
       <c r="H61" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B62" s="10" t="str">
         <f aca="false">LEFT(A62, FIND("_", A62, 1) - 1)</f>
@@ -12346,19 +12358,19 @@
         <v>79</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H62" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B63" s="10" t="str">
         <f aca="false">LEFT(A63, FIND("_", A63, 1) - 1)</f>
@@ -12373,19 +12385,19 @@
         <v>79</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H63" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B64" s="10" t="str">
         <f aca="false">LEFT(A64, FIND("_", A64, 1) - 1)</f>
@@ -12400,19 +12412,19 @@
         <v>79</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G64" s="10" t="s">
         <v>111</v>
       </c>
       <c r="H64" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B65" s="10" t="str">
         <f aca="false">LEFT(A65, FIND("_", A65, 1) - 1)</f>
@@ -12427,19 +12439,19 @@
         <v>79</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>105</v>
       </c>
       <c r="H65" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="10" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B66" s="10" t="str">
         <f aca="false">LEFT(A66, FIND("_", A66, 1) - 1)</f>
@@ -12454,19 +12466,19 @@
         <v>79</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>107</v>
       </c>
       <c r="H66" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B67" s="10" t="str">
         <f aca="false">LEFT(A67, FIND("_", A67, 1) - 1)</f>
@@ -12481,19 +12493,19 @@
         <v>79</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H67" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B68" s="10" t="str">
         <f aca="false">LEFT(A68, FIND("_", A68, 1) - 1)</f>
@@ -12508,19 +12520,19 @@
         <v>79</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>113</v>
       </c>
       <c r="H68" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="10" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B69" s="10" t="str">
         <f aca="false">LEFT(A69, FIND("_", A69, 1) - 1)</f>
@@ -12535,19 +12547,19 @@
         <v>79</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G69" s="10" t="s">
         <v>140</v>
       </c>
       <c r="H69" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B70" s="10" t="str">
         <f aca="false">LEFT(A70, FIND("_", A70, 1) - 1)</f>
@@ -12562,119 +12574,119 @@
         <v>79</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G70" s="10" t="s">
         <v>142</v>
       </c>
       <c r="H70" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B71" s="0"/>
       <c r="C71" s="0"/>
       <c r="D71" s="0"/>
       <c r="E71" s="0"/>
       <c r="F71" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>145</v>
       </c>
       <c r="H71" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I71" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B72" s="0"/>
       <c r="C72" s="0"/>
       <c r="D72" s="0"/>
       <c r="E72" s="0"/>
       <c r="F72" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>62</v>
       </c>
       <c r="H72" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B73" s="0"/>
       <c r="C73" s="0"/>
       <c r="D73" s="0"/>
       <c r="E73" s="0"/>
       <c r="F73" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>88</v>
       </c>
       <c r="H73" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="10" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B74" s="0"/>
       <c r="C74" s="0"/>
       <c r="D74" s="0"/>
       <c r="E74" s="0"/>
       <c r="F74" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G74" s="10" t="s">
         <v>90</v>
       </c>
       <c r="H74" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B75" s="0"/>
       <c r="C75" s="0"/>
       <c r="D75" s="0"/>
       <c r="E75" s="0"/>
       <c r="F75" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>93</v>
       </c>
       <c r="H75" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="10" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B76" s="10" t="str">
         <f aca="false">LEFT(A76, FIND("_", A76, 1) - 1)</f>
         <v>28338</v>
       </c>
       <c r="C76" s="63" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D76" s="10" t="str">
         <f aca="false">RIGHT(A76, LEN(A76) - FIND("_", A76) - 3)</f>
@@ -12684,25 +12696,25 @@
         <v>79</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G76" s="10" t="s">
         <v>72</v>
       </c>
       <c r="H76" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="10" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B77" s="10" t="str">
         <f aca="false">LEFT(A77, FIND("_", A77, 1) - 1)</f>
         <v>29698</v>
       </c>
       <c r="C77" s="63" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D77" s="10" t="str">
         <f aca="false">RIGHT(A77, LEN(A77) - FIND("_", A77) - 3)</f>
@@ -12712,18 +12724,18 @@
         <v>79</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G77" s="10" t="s">
         <v>76</v>
       </c>
       <c r="H77" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B78" s="10" t="str">
         <f aca="false">LEFT(A78, FIND("_", A78, 1) - 1)</f>
@@ -12738,18 +12750,18 @@
         <v>79</v>
       </c>
       <c r="F78" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G78" s="10" t="s">
         <v>102</v>
       </c>
       <c r="H78" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="10" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B79" s="10" t="str">
         <f aca="false">LEFT(A79, FIND("_", A79, 1) - 1)</f>
@@ -12764,18 +12776,18 @@
         <v>79</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H79" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="10" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B80" s="10" t="str">
         <f aca="false">LEFT(A80, FIND("_", A80, 1) - 1)</f>
@@ -12790,18 +12802,18 @@
         <v>79</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H80" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="10" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B81" s="10" t="str">
         <f aca="false">LEFT(A81, FIND("_", A81, 1) - 1)</f>
@@ -12816,18 +12828,18 @@
         <v>79</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G81" s="10" t="s">
         <v>129</v>
       </c>
       <c r="H81" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="10" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B82" s="10" t="str">
         <f aca="false">LEFT(A82, FIND("_", A82, 1) - 1)</f>
@@ -12842,18 +12854,18 @@
         <v>79</v>
       </c>
       <c r="F82" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G82" s="10" t="s">
         <v>157</v>
       </c>
       <c r="H82" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="10" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B83" s="10" t="str">
         <f aca="false">LEFT(A83, FIND("_", A83, 1) - 1)</f>
@@ -12868,18 +12880,18 @@
         <v>79</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H83" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B84" s="10" t="str">
         <f aca="false">LEFT(A84, FIND("_", A84, 1) - 1)</f>
@@ -12894,18 +12906,18 @@
         <v>79</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H84" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="10" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B85" s="10" t="str">
         <f aca="false">LEFT(A85, FIND("_", A85, 1) - 1)</f>
@@ -12920,18 +12932,18 @@
         <v>79</v>
       </c>
       <c r="F85" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G85" s="10" t="s">
         <v>111</v>
       </c>
       <c r="H85" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B86" s="10" t="str">
         <f aca="false">LEFT(A86, FIND("_", A86, 1) - 1)</f>
@@ -12946,18 +12958,18 @@
         <v>79</v>
       </c>
       <c r="F86" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G86" s="10" t="s">
         <v>105</v>
       </c>
       <c r="H86" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B87" s="10" t="str">
         <f aca="false">LEFT(A87, FIND("_", A87, 1) - 1)</f>
@@ -12972,18 +12984,18 @@
         <v>79</v>
       </c>
       <c r="F87" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G87" s="10" t="s">
         <v>107</v>
       </c>
       <c r="H87" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B88" s="10" t="str">
         <f aca="false">LEFT(A88, FIND("_", A88, 1) - 1)</f>
@@ -12998,18 +13010,18 @@
         <v>79</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H88" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B89" s="10" t="str">
         <f aca="false">LEFT(A89, FIND("_", A89, 1) - 1)</f>
@@ -13024,18 +13036,18 @@
         <v>79</v>
       </c>
       <c r="F89" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>113</v>
       </c>
       <c r="H89" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="10" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B90" s="10" t="str">
         <f aca="false">LEFT(A90, FIND("_", A90, 1) - 1)</f>
@@ -13050,18 +13062,18 @@
         <v>79</v>
       </c>
       <c r="F90" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G90" s="10" t="s">
         <v>140</v>
       </c>
       <c r="H90" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="10" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B91" s="10" t="str">
         <f aca="false">LEFT(A91, FIND("_", A91, 1) - 1)</f>
@@ -13076,18 +13088,18 @@
         <v>79</v>
       </c>
       <c r="F91" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G91" s="10" t="s">
         <v>142</v>
       </c>
       <c r="H91" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B92" s="10" t="str">
         <f aca="false">LEFT(A92, FIND("_", A92, 1) - 1)</f>
@@ -13102,18 +13114,18 @@
         <v>79</v>
       </c>
       <c r="F92" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G92" s="10" t="s">
         <v>102</v>
       </c>
       <c r="H92" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="10" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B93" s="10" t="str">
         <f aca="false">LEFT(A93, FIND("_", A93, 1) - 1)</f>
@@ -13128,18 +13140,18 @@
         <v>79</v>
       </c>
       <c r="F93" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H93" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="10" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B94" s="10" t="str">
         <f aca="false">LEFT(A94, FIND("_", A94, 1) - 1)</f>
@@ -13154,18 +13166,18 @@
         <v>79</v>
       </c>
       <c r="F94" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H94" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="10" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B95" s="10" t="str">
         <f aca="false">LEFT(A95, FIND("_", A95, 1) - 1)</f>
@@ -13180,18 +13192,18 @@
         <v>79</v>
       </c>
       <c r="F95" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G95" s="10" t="s">
         <v>129</v>
       </c>
       <c r="H95" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="10" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B96" s="10" t="str">
         <f aca="false">LEFT(A96, FIND("_", A96, 1) - 1)</f>
@@ -13206,18 +13218,18 @@
         <v>79</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G96" s="10" t="s">
         <v>157</v>
       </c>
       <c r="H96" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="10" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B97" s="10" t="str">
         <f aca="false">LEFT(A97, FIND("_", A97, 1) - 1)</f>
@@ -13232,18 +13244,18 @@
         <v>79</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H97" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B98" s="10" t="str">
         <f aca="false">LEFT(A98, FIND("_", A98, 1) - 1)</f>
@@ -13258,18 +13270,18 @@
         <v>79</v>
       </c>
       <c r="F98" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G98" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H98" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B99" s="10" t="str">
         <f aca="false">LEFT(A99, FIND("_", A99, 1) - 1)</f>
@@ -13284,18 +13296,18 @@
         <v>79</v>
       </c>
       <c r="F99" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G99" s="10" t="s">
         <v>111</v>
       </c>
       <c r="H99" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B100" s="10" t="str">
         <f aca="false">LEFT(A100, FIND("_", A100, 1) - 1)</f>
@@ -13310,18 +13322,18 @@
         <v>79</v>
       </c>
       <c r="F100" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G100" s="10" t="s">
         <v>105</v>
       </c>
       <c r="H100" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B101" s="10" t="str">
         <f aca="false">LEFT(A101, FIND("_", A101, 1) - 1)</f>
@@ -13336,18 +13348,18 @@
         <v>79</v>
       </c>
       <c r="F101" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G101" s="10" t="s">
         <v>107</v>
       </c>
       <c r="H101" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B102" s="10" t="str">
         <f aca="false">LEFT(A102, FIND("_", A102, 1) - 1)</f>
@@ -13362,18 +13374,18 @@
         <v>79</v>
       </c>
       <c r="F102" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G102" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H102" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B103" s="10" t="str">
         <f aca="false">LEFT(A103, FIND("_", A103, 1) - 1)</f>
@@ -13388,18 +13400,18 @@
         <v>79</v>
       </c>
       <c r="F103" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G103" s="10" t="s">
         <v>113</v>
       </c>
       <c r="H103" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B104" s="10" t="str">
         <f aca="false">LEFT(A104, FIND("_", A104, 1) - 1)</f>
@@ -13414,18 +13426,18 @@
         <v>79</v>
       </c>
       <c r="F104" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G104" s="10" t="s">
         <v>140</v>
       </c>
       <c r="H104" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="10" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B105" s="10" t="str">
         <f aca="false">LEFT(A105, FIND("_", A105, 1) - 1)</f>
@@ -13440,18 +13452,18 @@
         <v>79</v>
       </c>
       <c r="F105" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G105" s="10" t="s">
         <v>142</v>
       </c>
       <c r="H105" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B106" s="10" t="str">
         <f aca="false">LEFT(A106, FIND("_", A106, 1) - 1)</f>
@@ -13466,18 +13478,18 @@
         <v>79</v>
       </c>
       <c r="F106" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G106" s="10" t="s">
         <v>102</v>
       </c>
       <c r="H106" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="10" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B107" s="10" t="str">
         <f aca="false">LEFT(A107, FIND("_", A107, 1) - 1)</f>
@@ -13492,18 +13504,18 @@
         <v>79</v>
       </c>
       <c r="F107" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H107" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="10" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B108" s="10" t="str">
         <f aca="false">LEFT(A108, FIND("_", A108, 1) - 1)</f>
@@ -13518,18 +13530,18 @@
         <v>79</v>
       </c>
       <c r="F108" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H108" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="10" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B109" s="10" t="str">
         <f aca="false">LEFT(A109, FIND("_", A109, 1) - 1)</f>
@@ -13541,21 +13553,21 @@
         <v>1</v>
       </c>
       <c r="E109" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F109" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G109" s="10" t="s">
         <v>129</v>
       </c>
       <c r="H109" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B110" s="10" t="str">
         <f aca="false">LEFT(A110, FIND("_", A110, 1) - 1)</f>
@@ -13567,21 +13579,21 @@
         <v>1</v>
       </c>
       <c r="E110" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F110" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G110" s="10" t="s">
         <v>132</v>
       </c>
       <c r="H110" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="10" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B111" s="10" t="str">
         <f aca="false">LEFT(A111, FIND("_", A111, 1) - 1)</f>
@@ -13593,21 +13605,21 @@
         <v>1</v>
       </c>
       <c r="E111" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F111" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G111" s="10" t="s">
         <v>134</v>
       </c>
       <c r="H111" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B112" s="10" t="str">
         <f aca="false">LEFT(A112, FIND("_", A112, 1) - 1)</f>
@@ -13619,21 +13631,21 @@
         <v>1</v>
       </c>
       <c r="E112" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F112" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G112" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H112" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B113" s="10" t="str">
         <f aca="false">LEFT(A113, FIND("_", A113, 1) - 1)</f>
@@ -13645,21 +13657,21 @@
         <v>1</v>
       </c>
       <c r="E113" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F113" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G113" s="10" t="s">
         <v>111</v>
       </c>
       <c r="H113" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B114" s="10" t="str">
         <f aca="false">LEFT(A114, FIND("_", A114, 1) - 1)</f>
@@ -13671,21 +13683,21 @@
         <v>1</v>
       </c>
       <c r="E114" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F114" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G114" s="10" t="s">
         <v>126</v>
       </c>
       <c r="H114" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B115" s="10" t="str">
         <f aca="false">LEFT(A115, FIND("_", A115, 1) - 1)</f>
@@ -13697,21 +13709,21 @@
         <v>1</v>
       </c>
       <c r="E115" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F115" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G115" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H115" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B116" s="10" t="str">
         <f aca="false">LEFT(A116, FIND("_", A116, 1) - 1)</f>
@@ -13723,21 +13735,21 @@
         <v>1</v>
       </c>
       <c r="E116" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F116" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G116" s="10" t="s">
         <v>157</v>
       </c>
       <c r="H116" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B117" s="10" t="str">
         <f aca="false">LEFT(A117, FIND("_", A117, 1) - 1)</f>
@@ -13749,21 +13761,21 @@
         <v>1</v>
       </c>
       <c r="E117" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F117" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G117" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H117" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B118" s="10" t="str">
         <f aca="false">LEFT(A118, FIND("_", A118, 1) - 1)</f>
@@ -13775,21 +13787,21 @@
         <v>1</v>
       </c>
       <c r="E118" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F118" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G118" s="10" t="s">
         <v>136</v>
       </c>
       <c r="H118" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B119" s="10" t="str">
         <f aca="false">LEFT(A119, FIND("_", A119, 1) - 1)</f>
@@ -13801,21 +13813,21 @@
         <v>1</v>
       </c>
       <c r="E119" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F119" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G119" s="10" t="s">
         <v>138</v>
       </c>
       <c r="H119" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B120" s="10" t="str">
         <f aca="false">LEFT(A120, FIND("_", A120, 1) - 1)</f>
@@ -13827,21 +13839,21 @@
         <v>1</v>
       </c>
       <c r="E120" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F120" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G120" s="10" t="s">
         <v>105</v>
       </c>
       <c r="H120" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B121" s="10" t="s">
         <v>21</v>
@@ -13852,21 +13864,21 @@
         <v>1</v>
       </c>
       <c r="E121" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F121" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G121" s="10" t="s">
         <v>107</v>
       </c>
       <c r="H121" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B122" s="10" t="s">
         <v>21</v>
@@ -13877,21 +13889,21 @@
         <v>1</v>
       </c>
       <c r="E122" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F122" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G122" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H122" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="10" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B123" s="10" t="n">
         <v>11686</v>
@@ -13902,21 +13914,21 @@
         <v>1</v>
       </c>
       <c r="E123" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F123" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G123" s="10" t="s">
         <v>155</v>
       </c>
       <c r="H123" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B124" s="10" t="n">
         <v>11686</v>
@@ -13927,21 +13939,21 @@
         <v>1</v>
       </c>
       <c r="E124" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F124" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G124" s="10" t="s">
         <v>140</v>
       </c>
       <c r="H124" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B125" s="10" t="n">
         <v>21665</v>
@@ -13952,21 +13964,21 @@
         <v>1</v>
       </c>
       <c r="E125" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F125" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G125" s="10" t="s">
         <v>142</v>
       </c>
       <c r="H125" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B126" s="10" t="n">
         <v>21665</v>
@@ -13977,21 +13989,21 @@
         <v>1</v>
       </c>
       <c r="E126" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F126" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G126" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H126" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B127" s="10" t="str">
         <f aca="false">LEFT(A127, FIND("_", A127, 1) - 1)</f>
@@ -14003,61 +14015,61 @@
         <v>1</v>
       </c>
       <c r="E127" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F127" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G127" s="10" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H127" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B128" s="0"/>
       <c r="C128" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D128" s="0"/>
       <c r="E128" s="0"/>
       <c r="F128" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G128" s="10" t="s">
         <v>109</v>
       </c>
       <c r="H128" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="10" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B129" s="0"/>
       <c r="C129" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D129" s="0"/>
       <c r="E129" s="0"/>
       <c r="F129" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G129" s="10" t="s">
         <v>113</v>
       </c>
       <c r="H129" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B130" s="10" t="str">
         <f aca="false">LEFT(A130, FIND("_", A130, 1) - 1)</f>
@@ -14071,18 +14083,18 @@
         <v>79</v>
       </c>
       <c r="F130" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G130" s="10" t="s">
         <v>102</v>
       </c>
       <c r="H130" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B131" s="10" t="str">
         <f aca="false">LEFT(A131, FIND("_", A131, 1) - 1)</f>
@@ -14096,18 +14108,18 @@
         <v>79</v>
       </c>
       <c r="F131" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G131" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H131" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B132" s="10" t="str">
         <f aca="false">LEFT(A132, FIND("_", A132, 1) - 1)</f>
@@ -14121,18 +14133,18 @@
         <v>79</v>
       </c>
       <c r="F132" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G132" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H132" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B133" s="10" t="str">
         <f aca="false">LEFT(A133, FIND("_", A133, 1) - 1)</f>
@@ -14143,21 +14155,21 @@
         <v>1</v>
       </c>
       <c r="E133" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F133" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G133" s="10" t="s">
         <v>129</v>
       </c>
       <c r="H133" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B134" s="10" t="str">
         <f aca="false">LEFT(A134, FIND("_", A134, 1) - 1)</f>
@@ -14168,21 +14180,21 @@
         <v>1</v>
       </c>
       <c r="E134" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F134" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G134" s="10" t="s">
         <v>132</v>
       </c>
       <c r="H134" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="10" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B135" s="10" t="str">
         <f aca="false">LEFT(A135, FIND("_", A135, 1) - 1)</f>
@@ -14193,21 +14205,21 @@
         <v>1</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F135" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G135" s="10" t="s">
         <v>134</v>
       </c>
       <c r="H135" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B136" s="10" t="str">
         <f aca="false">LEFT(A136, FIND("_", A136, 1) - 1)</f>
@@ -14218,21 +14230,21 @@
         <v>1</v>
       </c>
       <c r="E136" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F136" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G136" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H136" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="10" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B137" s="10" t="str">
         <f aca="false">LEFT(A137, FIND("_", A137, 1) - 1)</f>
@@ -14243,21 +14255,21 @@
         <v>1</v>
       </c>
       <c r="E137" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F137" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G137" s="10" t="s">
         <v>111</v>
       </c>
       <c r="H137" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="10" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B138" s="10" t="str">
         <f aca="false">LEFT(A138, FIND("_", A138, 1) - 1)</f>
@@ -14268,21 +14280,21 @@
         <v>1</v>
       </c>
       <c r="E138" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F138" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G138" s="10" t="s">
         <v>126</v>
       </c>
       <c r="H138" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B139" s="10" t="str">
         <f aca="false">LEFT(A139, FIND("_", A139, 1) - 1)</f>
@@ -14293,21 +14305,21 @@
         <v>1</v>
       </c>
       <c r="E139" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F139" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G139" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H139" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="10" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B140" s="10" t="str">
         <f aca="false">LEFT(A140, FIND("_", A140, 1) - 1)</f>
@@ -14318,21 +14330,21 @@
         <v>1</v>
       </c>
       <c r="E140" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F140" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G140" s="10" t="s">
         <v>157</v>
       </c>
       <c r="H140" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="10" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B141" s="10" t="str">
         <f aca="false">LEFT(A141, FIND("_", A141, 1) - 1)</f>
@@ -14343,21 +14355,21 @@
         <v>1</v>
       </c>
       <c r="E141" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F141" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G141" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H141" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B142" s="10" t="str">
         <f aca="false">LEFT(A142, FIND("_", A142, 1) - 1)</f>
@@ -14368,21 +14380,21 @@
         <v>1</v>
       </c>
       <c r="E142" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F142" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G142" s="10" t="s">
         <v>136</v>
       </c>
       <c r="H142" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="10" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B143" s="10" t="str">
         <f aca="false">LEFT(A143, FIND("_", A143, 1) - 1)</f>
@@ -14393,21 +14405,21 @@
         <v>1</v>
       </c>
       <c r="E143" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F143" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G143" s="10" t="s">
         <v>138</v>
       </c>
       <c r="H143" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="10" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B144" s="10" t="str">
         <f aca="false">LEFT(A144, FIND("_", A144, 1) - 1)</f>
@@ -14418,21 +14430,21 @@
         <v>1</v>
       </c>
       <c r="E144" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F144" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G144" s="10" t="s">
         <v>105</v>
       </c>
       <c r="H144" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B145" s="10" t="s">
         <v>21</v>
@@ -14442,21 +14454,21 @@
         <v>1</v>
       </c>
       <c r="E145" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F145" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G145" s="10" t="s">
         <v>107</v>
       </c>
       <c r="H145" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="10" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B146" s="10" t="s">
         <v>21</v>
@@ -14466,21 +14478,21 @@
         <v>1</v>
       </c>
       <c r="E146" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F146" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G146" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H146" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B147" s="10" t="n">
         <v>11686</v>
@@ -14490,21 +14502,21 @@
         <v>1</v>
       </c>
       <c r="E147" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F147" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G147" s="10" t="s">
         <v>155</v>
       </c>
       <c r="H147" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="10" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B148" s="10" t="n">
         <v>11686</v>
@@ -14514,21 +14526,21 @@
         <v>1</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F148" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G148" s="10" t="s">
         <v>140</v>
       </c>
       <c r="H148" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="10" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B149" s="10" t="n">
         <v>21665</v>
@@ -14538,21 +14550,21 @@
         <v>1</v>
       </c>
       <c r="E149" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F149" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G149" s="10" t="s">
         <v>142</v>
       </c>
       <c r="H149" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="10" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B150" s="10" t="n">
         <v>21665</v>
@@ -14562,21 +14574,21 @@
         <v>1</v>
       </c>
       <c r="E150" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F150" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G150" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H150" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B151" s="10" t="str">
         <f aca="false">LEFT(A151, FIND("_", A151, 1) - 1)</f>
@@ -14587,50 +14599,50 @@
         <v>1</v>
       </c>
       <c r="E151" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F151" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G151" s="10" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H151" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="10" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C152" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F152" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G152" s="10" t="s">
         <v>109</v>
       </c>
       <c r="H152" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F153" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G153" s="10" t="s">
         <v>113</v>
       </c>
       <c r="H153" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -14653,7 +14665,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="1" sqref="C76:C77 E11"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -14672,29 +14684,29 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" s="63" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="63" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C2" s="63" t="n">
         <v>6</v>
       </c>
       <c r="D2" s="63" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B3" s="64" t="n">
         <v>41541</v>
@@ -14703,15 +14715,15 @@
         <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B4" s="64" t="n">
         <v>41626</v>
@@ -14720,15 +14732,15 @@
         <v>6</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B5" s="64" t="n">
         <v>41668</v>
@@ -14737,15 +14749,15 @@
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B6" s="64" t="n">
         <v>41680</v>
@@ -14754,15 +14766,15 @@
         <v>6</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B7" s="64" t="n">
         <v>41708</v>
@@ -14771,15 +14783,15 @@
         <v>12</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B8" s="64" t="n">
         <v>41731</v>
@@ -14788,15 +14800,15 @@
         <v>4</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B9" s="64" t="n">
         <v>41753</v>
@@ -14805,15 +14817,15 @@
         <v>12</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B10" s="64" t="n">
         <v>41792</v>
@@ -14822,15 +14834,15 @@
         <v>27</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B11" s="64" t="n">
         <v>41807</v>
@@ -14839,7 +14851,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -14862,7 +14874,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="1" sqref="C76:C77 H18"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -14885,13 +14897,13 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>58</v>
@@ -14900,7 +14912,7 @@
         <v>14</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14914,17 +14926,17 @@
         <v>500</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E2" s="7" t="n">
         <v>6</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G2" s="0"/>
       <c r="H2" s="7" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14938,17 +14950,17 @@
         <v>500</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E3" s="7" t="n">
         <v>9</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G3" s="0"/>
       <c r="H3" s="7" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14962,17 +14974,17 @@
         <v>600</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E4" s="7" t="n">
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="G4" s="0"/>
       <c r="H4" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14986,17 +14998,17 @@
         <v>602</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E5" s="7" t="n">
         <v>6</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G5" s="0"/>
       <c r="H5" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15010,17 +15022,17 @@
         <v>602</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E6" s="7" t="n">
         <v>8</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="G6" s="0"/>
       <c r="H6" s="7" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15034,17 +15046,17 @@
         <v>600</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E7" s="7" t="n">
         <v>9</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="G7" s="0"/>
       <c r="H7" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15058,24 +15070,24 @@
         <v>600</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E8" s="7" t="n">
         <v>4</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B9" s="64" t="n">
         <v>41710</v>
@@ -15084,16 +15096,16 @@
         <v>600</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E9" s="7" t="n">
         <v>7</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H9" s="0"/>
     </row>
@@ -15108,24 +15120,24 @@
         <v>600</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E10" s="7" t="n">
         <v>7</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B11" s="64" t="n">
         <v>41738</v>
@@ -15134,22 +15146,22 @@
         <v>600</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E11" s="7" t="n">
         <v>4</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G11" s="0"/>
       <c r="H11" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B12" s="64" t="n">
         <v>41759</v>
@@ -15158,22 +15170,22 @@
         <v>600</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E12" s="7" t="n">
         <v>14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="G12" s="0"/>
       <c r="H12" s="7" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B13" s="64" t="n">
         <v>41771</v>
@@ -15182,22 +15194,22 @@
         <v>600</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E13" s="7" t="n">
         <v>7</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="G13" s="0"/>
       <c r="H13" s="7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B14" s="64" t="n">
         <v>41779</v>
@@ -15206,24 +15218,24 @@
         <v>500</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E14" s="7" t="n">
         <v>14</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B15" s="64" t="n">
         <v>41784</v>
@@ -15232,24 +15244,24 @@
         <v>600</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E15" s="7" t="n">
         <v>14</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B16" s="64" t="n">
         <v>41801</v>
@@ -15258,24 +15270,24 @@
         <v>600</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E16" s="7" t="n">
         <v>24</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B17" s="64" t="n">
         <v>41807</v>
@@ -15284,19 +15296,19 @@
         <v>500</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E17" s="7" t="n">
         <v>24</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Little changes here and there
</commit_message>
<xml_diff>
--- a/hivwholeseq/tables/HIV_reservoir_all.xlsx
+++ b/hivwholeseq/tables/HIV_reservoir_all.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="457" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="457" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" state="visible" r:id="rId2"/>
@@ -1652,7 +1652,7 @@
     <t>VL98-1523</t>
   </si>
   <si>
-    <t>2 5</t>
+    <t>2 5a</t>
   </si>
   <si>
     <t>VK99-4204-F2_PCR1-2</t>
@@ -2595,8 +2595,8 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_15319" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_15319" xfId="21" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3485,14 +3485,15 @@
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -15126,8 +15127,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -15140,7 +15141,7 @@
   </sheetPr>
   <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M52" activeCellId="0" sqref="M52"/>
     </sheetView>
   </sheetViews>
@@ -19721,8 +19722,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -19735,8 +19736,8 @@
   </sheetPr>
   <dimension ref="A1:K238"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A172" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J235" activeCellId="0" sqref="J235"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A192" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E238" activeCellId="0" sqref="E238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -25094,6 +25095,7 @@
       <c r="B211" s="16" t="n">
         <v>28541</v>
       </c>
+      <c r="C211" s="0"/>
       <c r="D211" s="16" t="n">
         <v>1</v>
       </c>
@@ -25117,6 +25119,7 @@
       <c r="B212" s="16" t="n">
         <v>25268</v>
       </c>
+      <c r="C212" s="0"/>
       <c r="D212" s="16" t="n">
         <v>1</v>
       </c>
@@ -25140,6 +25143,7 @@
       <c r="B213" s="16" t="n">
         <v>5651</v>
       </c>
+      <c r="C213" s="0"/>
       <c r="D213" s="16" t="n">
         <v>1</v>
       </c>
@@ -25163,6 +25167,7 @@
       <c r="B214" s="16" t="n">
         <v>10110</v>
       </c>
+      <c r="C214" s="0"/>
       <c r="D214" s="16" t="n">
         <v>1</v>
       </c>
@@ -25186,6 +25191,7 @@
       <c r="B215" s="16" t="n">
         <v>3199</v>
       </c>
+      <c r="C215" s="0"/>
       <c r="D215" s="16" t="n">
         <v>1</v>
       </c>
@@ -25206,6 +25212,10 @@
       <c r="A216" s="82" t="s">
         <v>331</v>
       </c>
+      <c r="B216" s="0"/>
+      <c r="C216" s="0"/>
+      <c r="D216" s="0"/>
+      <c r="E216" s="0"/>
       <c r="F216" s="16" t="s">
         <v>497</v>
       </c>
@@ -25441,6 +25451,7 @@
       <c r="B226" s="16" t="n">
         <v>28541</v>
       </c>
+      <c r="C226" s="0"/>
       <c r="D226" s="16" t="n">
         <v>1</v>
       </c>
@@ -25464,6 +25475,7 @@
       <c r="B227" s="16" t="n">
         <v>25268</v>
       </c>
+      <c r="C227" s="0"/>
       <c r="D227" s="16" t="n">
         <v>1</v>
       </c>
@@ -25487,6 +25499,7 @@
       <c r="B228" s="16" t="n">
         <v>5651</v>
       </c>
+      <c r="C228" s="0"/>
       <c r="D228" s="16" t="n">
         <v>1</v>
       </c>
@@ -25510,6 +25523,7 @@
       <c r="B229" s="16" t="n">
         <v>10110</v>
       </c>
+      <c r="C229" s="0"/>
       <c r="D229" s="16" t="n">
         <v>1</v>
       </c>
@@ -25533,6 +25547,7 @@
       <c r="B230" s="16" t="n">
         <v>3199</v>
       </c>
+      <c r="C230" s="0"/>
       <c r="D230" s="16" t="n">
         <v>1</v>
       </c>
@@ -25580,7 +25595,7 @@
         <v>541</v>
       </c>
       <c r="B232" s="16" t="s">
-        <v>542</v>
+        <v>106</v>
       </c>
       <c r="C232" s="16" t="s">
         <v>542</v>
@@ -25743,6 +25758,9 @@
       </c>
       <c r="C238" s="16" t="n">
         <v>26585</v>
+      </c>
+      <c r="D238" s="16" t="n">
+        <v>1</v>
       </c>
       <c r="E238" s="16" t="s">
         <v>375</v>
@@ -25762,8 +25780,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -26604,8 +26622,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -26616,9 +26634,9 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E235"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -26845,6 +26863,7 @@
       <c r="D13" s="5" t="s">
         <v>610</v>
       </c>
+      <c r="E13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
@@ -26859,6 +26878,7 @@
       <c r="D14" s="5" t="s">
         <v>610</v>
       </c>
+      <c r="E14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
@@ -26881,13 +26901,15 @@
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -27475,8 +27497,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Propagators gene by gene (to be improved); distance from subtype
</commit_message>
<xml_diff>
--- a/hivwholeseq/tables/HIV_reservoir_all.xlsx
+++ b/hivwholeseq/tables/HIV_reservoir_all.xlsx
@@ -2595,8 +2595,8 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_15319" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_15319" xfId="21" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3492,8 +3492,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -15127,8 +15127,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -19722,8 +19722,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -19737,7 +19737,7 @@
   <dimension ref="A1:K238"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A192" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E238" activeCellId="0" sqref="E238"/>
+      <selection pane="topLeft" activeCell="G238" activeCellId="0" sqref="G238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -25780,8 +25780,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -26622,8 +26622,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -26908,8 +26908,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -27497,8 +27497,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HLA tries plus some improvement on to/from
</commit_message>
<xml_diff>
--- a/hivwholeseq/tables/HIV_reservoir_all.xlsx
+++ b/hivwholeseq/tables/HIV_reservoir_all.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="672" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="672" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" state="visible" r:id="rId2"/>
@@ -2309,7 +2309,7 @@
     <t>/ebio/abt6_sra/years/2014/06_23/HIVSwedenNexteraXTDualIndex/</t>
   </si>
   <si>
-    <t>16 pat samples + 1 THOMAS</t>
+    <t>16 pat samples (some with A. thaliana as buffer) + 1 THOMAS</t>
   </si>
   <si>
     <t>drop at read 300</t>
@@ -2665,7 +2665,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="115">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3050,10 +3050,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="18" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="169" fontId="18" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3138,12 +3134,12 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_15319" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1" xfId="22" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_15319" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Blad1" xfId="25" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -4034,8 +4030,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -13956,8 +13952,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -13969,7 +13965,7 @@
   </sheetPr>
   <dimension ref="A1:X106"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P4" activeCellId="0" sqref="P4"/>
     </sheetView>
   </sheetViews>
@@ -19492,7 +19488,7 @@
       <c r="E78" s="89"/>
       <c r="F78" s="89"/>
       <c r="G78" s="65"/>
-      <c r="H78" s="96"/>
+      <c r="H78" s="95"/>
       <c r="I78" s="68" t="s">
         <v>192</v>
       </c>
@@ -19704,7 +19700,7 @@
       <c r="G81" s="65" t="n">
         <v>66.6666666666667</v>
       </c>
-      <c r="H81" s="97" t="s">
+      <c r="H81" s="96" t="s">
         <v>177</v>
       </c>
       <c r="I81" s="68" t="s">
@@ -20276,7 +20272,7 @@
       <c r="G89" s="65" t="n">
         <v>10933.3333333333</v>
       </c>
-      <c r="H89" s="98" t="s">
+      <c r="H89" s="97" t="s">
         <v>183</v>
       </c>
       <c r="I89" s="68" t="s">
@@ -20343,8 +20339,8 @@
       <c r="F90" s="74" t="n">
         <v>280</v>
       </c>
-      <c r="G90" s="99"/>
-      <c r="H90" s="97" t="s">
+      <c r="G90" s="98"/>
+      <c r="H90" s="96" t="s">
         <v>207</v>
       </c>
       <c r="I90" s="68" t="s">
@@ -20412,7 +20408,7 @@
       <c r="E91" s="74"/>
       <c r="F91" s="74"/>
       <c r="G91" s="65"/>
-      <c r="H91" s="97" t="s">
+      <c r="H91" s="96" t="s">
         <v>207</v>
       </c>
       <c r="I91" s="68" t="s">
@@ -20486,7 +20482,7 @@
       <c r="G92" s="65" t="n">
         <v>66.7333333333333</v>
       </c>
-      <c r="H92" s="98" t="s">
+      <c r="H92" s="97" t="s">
         <v>177</v>
       </c>
       <c r="I92" s="68" t="s">
@@ -20556,7 +20552,7 @@
       <c r="G93" s="65" t="n">
         <v>0</v>
       </c>
-      <c r="H93" s="100" t="s">
+      <c r="H93" s="99" t="s">
         <v>218</v>
       </c>
       <c r="I93" s="68" t="s">
@@ -20627,7 +20623,7 @@
       <c r="G94" s="65" t="n">
         <v>0</v>
       </c>
-      <c r="H94" s="97" t="s">
+      <c r="H94" s="96" t="s">
         <v>177</v>
       </c>
       <c r="I94" s="68" t="s">
@@ -20723,7 +20719,7 @@
       <c r="O95" s="65" t="s">
         <v>179</v>
       </c>
-      <c r="P95" s="101"/>
+      <c r="P95" s="100"/>
       <c r="Q95" s="65" t="s">
         <v>180</v>
       </c>
@@ -20894,26 +20890,26 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="102" t="n">
+      <c r="A98" s="101" t="n">
         <v>9985</v>
       </c>
-      <c r="B98" s="102" t="n">
+      <c r="B98" s="101" t="n">
         <v>15034</v>
       </c>
-      <c r="C98" s="103" t="n">
+      <c r="C98" s="102" t="n">
         <v>35241</v>
       </c>
-      <c r="D98" s="104" t="n">
+      <c r="D98" s="103" t="n">
         <v>2190.5</v>
       </c>
-      <c r="E98" s="102" t="n">
+      <c r="E98" s="101" t="n">
         <v>12000</v>
       </c>
       <c r="F98" s="74"/>
       <c r="G98" s="65" t="n">
         <v>800</v>
       </c>
-      <c r="H98" s="105" t="s">
+      <c r="H98" s="104" t="s">
         <v>181</v>
       </c>
       <c r="I98" s="68" t="s">
@@ -20964,26 +20960,26 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="102" t="n">
+      <c r="A99" s="101" t="n">
         <v>10110</v>
       </c>
-      <c r="B99" s="102" t="n">
+      <c r="B99" s="101" t="n">
         <v>15034</v>
       </c>
-      <c r="C99" s="103" t="n">
+      <c r="C99" s="102" t="n">
         <v>35268</v>
       </c>
-      <c r="D99" s="104" t="n">
+      <c r="D99" s="103" t="n">
         <v>2217.5</v>
       </c>
-      <c r="E99" s="102" t="n">
+      <c r="E99" s="101" t="n">
         <v>10500</v>
       </c>
       <c r="F99" s="74"/>
       <c r="G99" s="65" t="n">
         <v>700</v>
       </c>
-      <c r="H99" s="106" t="s">
+      <c r="H99" s="105" t="s">
         <v>177</v>
       </c>
       <c r="I99" s="68" t="s">
@@ -21342,7 +21338,7 @@
       <c r="G104" s="65" t="n">
         <v>4200</v>
       </c>
-      <c r="H104" s="107" t="s">
+      <c r="H104" s="106" t="s">
         <v>184</v>
       </c>
       <c r="I104" s="68" t="s">
@@ -21541,8 +21537,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -21575,43 +21571,43 @@
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57589285714286"/>
   </cols>
   <sheetData>
-    <row r="1" s="108" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="108" t="s">
+    <row r="1" s="107" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="107" t="s">
         <v>220</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="107" t="s">
         <v>221</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="107" t="s">
         <v>222</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="107" t="s">
         <v>223</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="F1" s="107" t="s">
         <v>224</v>
       </c>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="107" t="s">
         <v>225</v>
       </c>
-      <c r="H1" s="108" t="s">
+      <c r="H1" s="107" t="s">
         <v>226</v>
       </c>
-      <c r="I1" s="108" t="s">
+      <c r="I1" s="107" t="s">
         <v>227</v>
       </c>
-      <c r="J1" s="109" t="s">
+      <c r="J1" s="108" t="s">
         <v>103</v>
       </c>
-      <c r="K1" s="108" t="s">
+      <c r="K1" s="107" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="109" t="s">
         <v>229</v>
       </c>
       <c r="B2" s="0"/>
@@ -21634,7 +21630,7 @@
       <c r="I2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="109" t="s">
         <v>234</v>
       </c>
       <c r="B3" s="0"/>
@@ -21660,7 +21656,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="109" t="s">
         <v>237</v>
       </c>
       <c r="B4" s="0"/>
@@ -21683,7 +21679,7 @@
       <c r="I4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="110" t="n">
+      <c r="A5" s="109" t="n">
         <v>37024</v>
       </c>
       <c r="B5" s="0"/>
@@ -21708,7 +21704,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="109" t="s">
         <v>241</v>
       </c>
       <c r="B6" s="0"/>
@@ -21736,7 +21732,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="110" t="s">
+      <c r="A7" s="109" t="s">
         <v>245</v>
       </c>
       <c r="B7" s="0"/>
@@ -21764,7 +21760,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="110" t="s">
+      <c r="A8" s="109" t="s">
         <v>248</v>
       </c>
       <c r="B8" s="0"/>
@@ -21788,7 +21784,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="110" t="s">
+      <c r="A9" s="109" t="s">
         <v>253</v>
       </c>
       <c r="B9" s="0"/>
@@ -21812,7 +21808,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="110" t="s">
+      <c r="A10" s="109" t="s">
         <v>254</v>
       </c>
       <c r="B10" s="14" t="str">
@@ -21839,7 +21835,7 @@
       <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="110" t="s">
+      <c r="A11" s="109" t="s">
         <v>257</v>
       </c>
       <c r="B11" s="14" t="str">
@@ -21866,7 +21862,7 @@
       <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="110" t="s">
+      <c r="A12" s="109" t="s">
         <v>258</v>
       </c>
       <c r="B12" s="14" t="str">
@@ -21893,7 +21889,7 @@
       <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="110" t="s">
+      <c r="A13" s="109" t="s">
         <v>260</v>
       </c>
       <c r="B13" s="14" t="str">
@@ -21920,7 +21916,7 @@
       <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="110" t="s">
+      <c r="A14" s="109" t="s">
         <v>262</v>
       </c>
       <c r="B14" s="14" t="str">
@@ -21947,7 +21943,7 @@
       <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="109" t="s">
         <v>263</v>
       </c>
       <c r="B15" s="14" t="str">
@@ -21974,7 +21970,7 @@
       <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="110" t="s">
+      <c r="A16" s="109" t="s">
         <v>265</v>
       </c>
       <c r="B16" s="14" t="str">
@@ -22001,7 +21997,7 @@
       <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="110" t="s">
+      <c r="A17" s="109" t="s">
         <v>267</v>
       </c>
       <c r="B17" s="14" t="str">
@@ -22028,7 +22024,7 @@
       <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="110" t="s">
+      <c r="A18" s="109" t="s">
         <v>269</v>
       </c>
       <c r="B18" s="14" t="str">
@@ -22055,7 +22051,7 @@
       <c r="I18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="110" t="s">
+      <c r="A19" s="109" t="s">
         <v>271</v>
       </c>
       <c r="B19" s="0"/>
@@ -22079,7 +22075,7 @@
       <c r="I19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="110" t="s">
+      <c r="A20" s="109" t="s">
         <v>275</v>
       </c>
       <c r="B20" s="0"/>
@@ -22103,7 +22099,7 @@
       <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="110" t="s">
+      <c r="A21" s="109" t="s">
         <v>277</v>
       </c>
       <c r="B21" s="0"/>
@@ -22126,7 +22122,7 @@
       <c r="I21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="110" t="s">
+      <c r="A22" s="109" t="s">
         <v>279</v>
       </c>
       <c r="B22" s="0"/>
@@ -22149,7 +22145,7 @@
       <c r="I22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="110" t="s">
+      <c r="A23" s="109" t="s">
         <v>281</v>
       </c>
       <c r="B23" s="0"/>
@@ -22172,7 +22168,7 @@
       <c r="I23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="110" t="s">
+      <c r="A24" s="109" t="s">
         <v>283</v>
       </c>
       <c r="B24" s="0"/>
@@ -22195,7 +22191,7 @@
       <c r="I24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="110" t="s">
+      <c r="A25" s="109" t="s">
         <v>285</v>
       </c>
       <c r="B25" s="0"/>
@@ -22218,7 +22214,7 @@
       <c r="I25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="110" t="s">
+      <c r="A26" s="109" t="s">
         <v>287</v>
       </c>
       <c r="B26" s="0"/>
@@ -22241,7 +22237,7 @@
       <c r="I26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="109" t="s">
         <v>288</v>
       </c>
       <c r="B27" s="14" t="str">
@@ -22268,7 +22264,7 @@
       <c r="I27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="110" t="s">
+      <c r="A28" s="109" t="s">
         <v>289</v>
       </c>
       <c r="B28" s="14" t="str">
@@ -22295,7 +22291,7 @@
       <c r="I28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="110" t="s">
+      <c r="A29" s="109" t="s">
         <v>290</v>
       </c>
       <c r="B29" s="14" t="str">
@@ -22322,7 +22318,7 @@
       <c r="I29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="110" t="s">
+      <c r="A30" s="109" t="s">
         <v>291</v>
       </c>
       <c r="B30" s="14" t="str">
@@ -22349,7 +22345,7 @@
       <c r="I30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="110" t="s">
+      <c r="A31" s="109" t="s">
         <v>292</v>
       </c>
       <c r="B31" s="14" t="str">
@@ -22376,7 +22372,7 @@
       <c r="I31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="110" t="s">
+      <c r="A32" s="109" t="s">
         <v>293</v>
       </c>
       <c r="B32" s="14" t="str">
@@ -22403,7 +22399,7 @@
       <c r="I32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="110" t="s">
+      <c r="A33" s="109" t="s">
         <v>294</v>
       </c>
       <c r="B33" s="0"/>
@@ -22426,7 +22422,7 @@
       <c r="I33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="110" t="s">
+      <c r="A34" s="109" t="s">
         <v>296</v>
       </c>
       <c r="B34" s="0"/>
@@ -22449,7 +22445,7 @@
       <c r="I34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="110" t="s">
+      <c r="A35" s="109" t="s">
         <v>298</v>
       </c>
       <c r="B35" s="0"/>
@@ -22472,7 +22468,7 @@
       <c r="I35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="110" t="s">
+      <c r="A36" s="109" t="s">
         <v>302</v>
       </c>
       <c r="B36" s="0"/>
@@ -22495,7 +22491,7 @@
       <c r="I36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="110" t="s">
+      <c r="A37" s="109" t="s">
         <v>304</v>
       </c>
       <c r="B37" s="0"/>
@@ -22518,7 +22514,7 @@
       <c r="I37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="110" t="s">
+      <c r="A38" s="109" t="s">
         <v>306</v>
       </c>
       <c r="B38" s="0"/>
@@ -22541,7 +22537,7 @@
       <c r="I38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="110" t="s">
+      <c r="A39" s="109" t="s">
         <v>308</v>
       </c>
       <c r="B39" s="14" t="str">
@@ -22568,7 +22564,7 @@
       <c r="I39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="110" t="s">
+      <c r="A40" s="109" t="s">
         <v>310</v>
       </c>
       <c r="B40" s="14" t="str">
@@ -22595,7 +22591,7 @@
       <c r="I40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="110" t="s">
+      <c r="A41" s="109" t="s">
         <v>312</v>
       </c>
       <c r="B41" s="14" t="str">
@@ -22622,7 +22618,7 @@
       <c r="I41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="110" t="s">
+      <c r="A42" s="109" t="s">
         <v>314</v>
       </c>
       <c r="B42" s="0"/>
@@ -22643,7 +22639,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="110" t="s">
+      <c r="A43" s="109" t="s">
         <v>319</v>
       </c>
       <c r="B43" s="14" t="str">
@@ -22670,7 +22666,7 @@
       <c r="I43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="110" t="s">
+      <c r="A44" s="109" t="s">
         <v>321</v>
       </c>
       <c r="B44" s="14" t="str">
@@ -22697,7 +22693,7 @@
       <c r="I44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="110" t="s">
+      <c r="A45" s="109" t="s">
         <v>322</v>
       </c>
       <c r="B45" s="14" t="str">
@@ -22724,7 +22720,7 @@
       <c r="I45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="110" t="s">
+      <c r="A46" s="109" t="s">
         <v>323</v>
       </c>
       <c r="B46" s="0"/>
@@ -22745,7 +22741,7 @@
       <c r="I46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="110" t="n">
+      <c r="A47" s="109" t="n">
         <v>38540</v>
       </c>
       <c r="B47" s="0"/>
@@ -22766,7 +22762,7 @@
       <c r="I47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="110" t="n">
+      <c r="A48" s="109" t="n">
         <v>38304</v>
       </c>
       <c r="B48" s="0"/>
@@ -22787,7 +22783,7 @@
       <c r="I48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="110" t="s">
+      <c r="A49" s="109" t="s">
         <v>327</v>
       </c>
       <c r="B49" s="14" t="str">
@@ -22817,7 +22813,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="110" t="s">
+      <c r="A50" s="109" t="s">
         <v>330</v>
       </c>
       <c r="B50" s="14" t="str">
@@ -22847,7 +22843,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="110" t="s">
+      <c r="A51" s="109" t="s">
         <v>332</v>
       </c>
       <c r="B51" s="14" t="str">
@@ -22874,7 +22870,7 @@
       <c r="I51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="110" t="s">
+      <c r="A52" s="109" t="s">
         <v>334</v>
       </c>
       <c r="B52" s="14" t="str">
@@ -22901,7 +22897,7 @@
       <c r="I52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="110" t="s">
+      <c r="A53" s="109" t="s">
         <v>335</v>
       </c>
       <c r="B53" s="0"/>
@@ -22922,7 +22918,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="110" t="s">
+      <c r="A54" s="109" t="s">
         <v>338</v>
       </c>
       <c r="B54" s="14" t="str">
@@ -22950,7 +22946,7 @@
       <c r="I54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="110" t="s">
+      <c r="A55" s="109" t="s">
         <v>340</v>
       </c>
       <c r="B55" s="14" t="str">
@@ -22978,7 +22974,7 @@
       <c r="I55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="110" t="s">
+      <c r="A56" s="109" t="s">
         <v>342</v>
       </c>
       <c r="B56" s="14" t="str">
@@ -23006,7 +23002,7 @@
       <c r="I56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="110" t="s">
+      <c r="A57" s="109" t="s">
         <v>344</v>
       </c>
       <c r="B57" s="14" t="str">
@@ -23033,7 +23029,7 @@
       <c r="I57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="110" t="s">
+      <c r="A58" s="109" t="s">
         <v>347</v>
       </c>
       <c r="B58" s="14" t="str">
@@ -23060,7 +23056,7 @@
       <c r="I58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="110" t="s">
+      <c r="A59" s="109" t="s">
         <v>349</v>
       </c>
       <c r="B59" s="14" t="str">
@@ -23087,7 +23083,7 @@
       <c r="I59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="110" t="s">
+      <c r="A60" s="109" t="s">
         <v>352</v>
       </c>
       <c r="B60" s="14" t="str">
@@ -23114,7 +23110,7 @@
       <c r="I60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="110" t="s">
+      <c r="A61" s="109" t="s">
         <v>353</v>
       </c>
       <c r="B61" s="14" t="str">
@@ -23141,7 +23137,7 @@
       <c r="I61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="110" t="s">
+      <c r="A62" s="109" t="s">
         <v>354</v>
       </c>
       <c r="B62" s="14" t="str">
@@ -23168,7 +23164,7 @@
       <c r="I62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="110" t="s">
+      <c r="A63" s="109" t="s">
         <v>356</v>
       </c>
       <c r="B63" s="14" t="str">
@@ -23195,7 +23191,7 @@
       <c r="I63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="110" t="s">
+      <c r="A64" s="109" t="s">
         <v>358</v>
       </c>
       <c r="B64" s="14" t="str">
@@ -23222,7 +23218,7 @@
       <c r="I64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="110" t="s">
+      <c r="A65" s="109" t="s">
         <v>359</v>
       </c>
       <c r="B65" s="14" t="str">
@@ -23249,7 +23245,7 @@
       <c r="I65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="110" t="s">
+      <c r="A66" s="109" t="s">
         <v>360</v>
       </c>
       <c r="B66" s="14" t="str">
@@ -23276,7 +23272,7 @@
       <c r="I66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="110" t="s">
+      <c r="A67" s="109" t="s">
         <v>361</v>
       </c>
       <c r="B67" s="14" t="str">
@@ -23303,7 +23299,7 @@
       <c r="I67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="110" t="s">
+      <c r="A68" s="109" t="s">
         <v>363</v>
       </c>
       <c r="B68" s="14" t="str">
@@ -23330,7 +23326,7 @@
       <c r="I68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="110" t="s">
+      <c r="A69" s="109" t="s">
         <v>364</v>
       </c>
       <c r="B69" s="14" t="str">
@@ -23357,7 +23353,7 @@
       <c r="I69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="110" t="s">
+      <c r="A70" s="109" t="s">
         <v>365</v>
       </c>
       <c r="B70" s="14" t="str">
@@ -23384,7 +23380,7 @@
       <c r="I70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="110" t="s">
+      <c r="A71" s="109" t="s">
         <v>366</v>
       </c>
       <c r="B71" s="0"/>
@@ -23405,7 +23401,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="110" t="s">
+      <c r="A72" s="109" t="s">
         <v>369</v>
       </c>
       <c r="B72" s="0"/>
@@ -23423,7 +23419,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="110" t="s">
+      <c r="A73" s="109" t="s">
         <v>371</v>
       </c>
       <c r="B73" s="0"/>
@@ -23441,7 +23437,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="110" t="s">
+      <c r="A74" s="109" t="s">
         <v>372</v>
       </c>
       <c r="B74" s="0"/>
@@ -23459,7 +23455,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="110" t="s">
+      <c r="A75" s="109" t="s">
         <v>373</v>
       </c>
       <c r="B75" s="0"/>
@@ -23477,7 +23473,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="110" t="s">
+      <c r="A76" s="109" t="s">
         <v>374</v>
       </c>
       <c r="B76" s="14" t="str">
@@ -23505,7 +23501,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="110" t="s">
+      <c r="A77" s="109" t="s">
         <v>376</v>
       </c>
       <c r="B77" s="14" t="str">
@@ -23533,7 +23529,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="110" t="s">
+      <c r="A78" s="109" t="s">
         <v>378</v>
       </c>
       <c r="B78" s="14" t="str">
@@ -23559,7 +23555,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="110" t="s">
+      <c r="A79" s="109" t="s">
         <v>380</v>
       </c>
       <c r="B79" s="14" t="str">
@@ -23585,7 +23581,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="110" t="s">
+      <c r="A80" s="109" t="s">
         <v>381</v>
       </c>
       <c r="B80" s="14" t="str">
@@ -23611,7 +23607,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="110" t="s">
+      <c r="A81" s="109" t="s">
         <v>382</v>
       </c>
       <c r="B81" s="14" t="str">
@@ -23637,7 +23633,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="110" t="s">
+      <c r="A82" s="109" t="s">
         <v>383</v>
       </c>
       <c r="B82" s="14" t="str">
@@ -23663,7 +23659,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="110" t="s">
+      <c r="A83" s="109" t="s">
         <v>384</v>
       </c>
       <c r="B83" s="14" t="str">
@@ -23689,7 +23685,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="110" t="s">
+      <c r="A84" s="109" t="s">
         <v>385</v>
       </c>
       <c r="B84" s="14" t="str">
@@ -23715,7 +23711,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="110" t="s">
+      <c r="A85" s="109" t="s">
         <v>386</v>
       </c>
       <c r="B85" s="14" t="str">
@@ -23741,7 +23737,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="110" t="s">
+      <c r="A86" s="109" t="s">
         <v>387</v>
       </c>
       <c r="B86" s="14" t="str">
@@ -23767,7 +23763,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="110" t="s">
+      <c r="A87" s="109" t="s">
         <v>388</v>
       </c>
       <c r="B87" s="14" t="str">
@@ -23793,7 +23789,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="110" t="s">
+      <c r="A88" s="109" t="s">
         <v>389</v>
       </c>
       <c r="B88" s="14" t="str">
@@ -23819,7 +23815,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="110" t="s">
+      <c r="A89" s="109" t="s">
         <v>390</v>
       </c>
       <c r="B89" s="14" t="str">
@@ -23845,7 +23841,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="110" t="s">
+      <c r="A90" s="109" t="s">
         <v>391</v>
       </c>
       <c r="B90" s="14" t="str">
@@ -23871,7 +23867,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="110" t="s">
+      <c r="A91" s="109" t="s">
         <v>392</v>
       </c>
       <c r="B91" s="14" t="str">
@@ -23897,7 +23893,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="110" t="s">
+      <c r="A92" s="109" t="s">
         <v>393</v>
       </c>
       <c r="B92" s="14" t="str">
@@ -23923,7 +23919,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="110" t="s">
+      <c r="A93" s="109" t="s">
         <v>395</v>
       </c>
       <c r="B93" s="14" t="str">
@@ -23949,7 +23945,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="110" t="s">
+      <c r="A94" s="109" t="s">
         <v>396</v>
       </c>
       <c r="B94" s="14" t="str">
@@ -23975,7 +23971,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="110" t="s">
+      <c r="A95" s="109" t="s">
         <v>397</v>
       </c>
       <c r="B95" s="14" t="str">
@@ -24001,7 +23997,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="110" t="s">
+      <c r="A96" s="109" t="s">
         <v>398</v>
       </c>
       <c r="B96" s="14" t="str">
@@ -24027,7 +24023,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="110" t="s">
+      <c r="A97" s="109" t="s">
         <v>399</v>
       </c>
       <c r="B97" s="14" t="str">
@@ -24053,7 +24049,7 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="110" t="s">
+      <c r="A98" s="109" t="s">
         <v>400</v>
       </c>
       <c r="B98" s="14" t="str">
@@ -24079,7 +24075,7 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="110" t="s">
+      <c r="A99" s="109" t="s">
         <v>401</v>
       </c>
       <c r="B99" s="14" t="str">
@@ -24105,7 +24101,7 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="110" t="s">
+      <c r="A100" s="109" t="s">
         <v>402</v>
       </c>
       <c r="B100" s="14" t="str">
@@ -24131,7 +24127,7 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="110" t="s">
+      <c r="A101" s="109" t="s">
         <v>403</v>
       </c>
       <c r="B101" s="14" t="str">
@@ -24157,7 +24153,7 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="110" t="s">
+      <c r="A102" s="109" t="s">
         <v>404</v>
       </c>
       <c r="B102" s="14" t="str">
@@ -24183,7 +24179,7 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="110" t="s">
+      <c r="A103" s="109" t="s">
         <v>405</v>
       </c>
       <c r="B103" s="14" t="str">
@@ -24209,7 +24205,7 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="110" t="s">
+      <c r="A104" s="109" t="s">
         <v>406</v>
       </c>
       <c r="B104" s="14" t="str">
@@ -24235,7 +24231,7 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="110" t="s">
+      <c r="A105" s="109" t="s">
         <v>407</v>
       </c>
       <c r="B105" s="14" t="str">
@@ -24261,7 +24257,7 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="110" t="s">
+      <c r="A106" s="109" t="s">
         <v>408</v>
       </c>
       <c r="B106" s="14" t="str">
@@ -24287,7 +24283,7 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="110" t="s">
+      <c r="A107" s="109" t="s">
         <v>411</v>
       </c>
       <c r="B107" s="14" t="str">
@@ -24313,7 +24309,7 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="110" t="s">
+      <c r="A108" s="109" t="s">
         <v>412</v>
       </c>
       <c r="B108" s="14" t="str">
@@ -24339,7 +24335,7 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="110" t="s">
+      <c r="A109" s="109" t="s">
         <v>413</v>
       </c>
       <c r="B109" s="14" t="str">
@@ -24365,7 +24361,7 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="110" t="s">
+      <c r="A110" s="109" t="s">
         <v>415</v>
       </c>
       <c r="B110" s="14" t="str">
@@ -24391,7 +24387,7 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="110" t="s">
+      <c r="A111" s="109" t="s">
         <v>416</v>
       </c>
       <c r="B111" s="14" t="str">
@@ -24417,7 +24413,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="110" t="s">
+      <c r="A112" s="109" t="s">
         <v>417</v>
       </c>
       <c r="B112" s="14" t="str">
@@ -24443,7 +24439,7 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="110" t="s">
+      <c r="A113" s="109" t="s">
         <v>419</v>
       </c>
       <c r="B113" s="14" t="str">
@@ -24469,7 +24465,7 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="110" t="s">
+      <c r="A114" s="109" t="s">
         <v>420</v>
       </c>
       <c r="B114" s="14" t="str">
@@ -24495,7 +24491,7 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="110" t="s">
+      <c r="A115" s="109" t="s">
         <v>421</v>
       </c>
       <c r="B115" s="14" t="str">
@@ -24521,7 +24517,7 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="110" t="s">
+      <c r="A116" s="109" t="s">
         <v>422</v>
       </c>
       <c r="B116" s="14" t="str">
@@ -24547,7 +24543,7 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="110" t="s">
+      <c r="A117" s="109" t="s">
         <v>423</v>
       </c>
       <c r="B117" s="14" t="str">
@@ -24573,7 +24569,7 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="110" t="s">
+      <c r="A118" s="109" t="s">
         <v>424</v>
       </c>
       <c r="B118" s="14" t="str">
@@ -24599,7 +24595,7 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="110" t="s">
+      <c r="A119" s="109" t="s">
         <v>425</v>
       </c>
       <c r="B119" s="14" t="str">
@@ -24625,7 +24621,7 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="110" t="s">
+      <c r="A120" s="109" t="s">
         <v>426</v>
       </c>
       <c r="B120" s="14" t="str">
@@ -24651,7 +24647,7 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="110" t="s">
+      <c r="A121" s="109" t="s">
         <v>427</v>
       </c>
       <c r="B121" s="14" t="s">
@@ -24676,7 +24672,7 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="110" t="s">
+      <c r="A122" s="109" t="s">
         <v>429</v>
       </c>
       <c r="B122" s="14" t="s">
@@ -24701,7 +24697,7 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="110" t="s">
+      <c r="A123" s="109" t="s">
         <v>431</v>
       </c>
       <c r="B123" s="14" t="n">
@@ -24726,7 +24722,7 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="110" t="s">
+      <c r="A124" s="109" t="s">
         <v>432</v>
       </c>
       <c r="B124" s="14" t="n">
@@ -24751,7 +24747,7 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="110" t="s">
+      <c r="A125" s="109" t="s">
         <v>433</v>
       </c>
       <c r="B125" s="14" t="n">
@@ -24776,7 +24772,7 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="110" t="s">
+      <c r="A126" s="109" t="s">
         <v>434</v>
       </c>
       <c r="B126" s="14" t="n">
@@ -24801,7 +24797,7 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="110" t="s">
+      <c r="A127" s="109" t="s">
         <v>435</v>
       </c>
       <c r="B127" s="14" t="str">
@@ -24827,7 +24823,7 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="110" t="s">
+      <c r="A128" s="109" t="s">
         <v>438</v>
       </c>
       <c r="B128" s="0"/>
@@ -24847,7 +24843,7 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="110" t="s">
+      <c r="A129" s="109" t="s">
         <v>440</v>
       </c>
       <c r="B129" s="0"/>
@@ -24867,7 +24863,7 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="110" t="s">
+      <c r="A130" s="109" t="s">
         <v>442</v>
       </c>
       <c r="B130" s="14" t="str">
@@ -24892,7 +24888,7 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="110" t="s">
+      <c r="A131" s="109" t="s">
         <v>444</v>
       </c>
       <c r="B131" s="14" t="str">
@@ -24917,7 +24913,7 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="110" t="s">
+      <c r="A132" s="109" t="s">
         <v>445</v>
       </c>
       <c r="B132" s="14" t="str">
@@ -24942,7 +24938,7 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="110" t="s">
+      <c r="A133" s="109" t="s">
         <v>446</v>
       </c>
       <c r="B133" s="14" t="str">
@@ -24967,7 +24963,7 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="110" t="s">
+      <c r="A134" s="109" t="s">
         <v>447</v>
       </c>
       <c r="B134" s="14" t="str">
@@ -24992,7 +24988,7 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="110" t="s">
+      <c r="A135" s="109" t="s">
         <v>448</v>
       </c>
       <c r="B135" s="14" t="str">
@@ -25017,7 +25013,7 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="110" t="s">
+      <c r="A136" s="109" t="s">
         <v>449</v>
       </c>
       <c r="B136" s="14" t="str">
@@ -25042,7 +25038,7 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="110" t="s">
+      <c r="A137" s="109" t="s">
         <v>450</v>
       </c>
       <c r="B137" s="14" t="str">
@@ -25067,7 +25063,7 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="110" t="s">
+      <c r="A138" s="109" t="s">
         <v>451</v>
       </c>
       <c r="B138" s="14" t="str">
@@ -25092,7 +25088,7 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="110" t="s">
+      <c r="A139" s="109" t="s">
         <v>452</v>
       </c>
       <c r="B139" s="14" t="str">
@@ -25117,7 +25113,7 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="110" t="s">
+      <c r="A140" s="109" t="s">
         <v>453</v>
       </c>
       <c r="B140" s="14" t="str">
@@ -25142,7 +25138,7 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="110" t="s">
+      <c r="A141" s="109" t="s">
         <v>454</v>
       </c>
       <c r="B141" s="14" t="str">
@@ -25167,7 +25163,7 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="110" t="s">
+      <c r="A142" s="109" t="s">
         <v>455</v>
       </c>
       <c r="B142" s="14" t="str">
@@ -25192,7 +25188,7 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="110" t="s">
+      <c r="A143" s="109" t="s">
         <v>456</v>
       </c>
       <c r="B143" s="14" t="str">
@@ -25217,7 +25213,7 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="110" t="s">
+      <c r="A144" s="109" t="s">
         <v>457</v>
       </c>
       <c r="B144" s="14" t="str">
@@ -25242,7 +25238,7 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="110" t="s">
+      <c r="A145" s="109" t="s">
         <v>458</v>
       </c>
       <c r="B145" s="14" t="s">
@@ -25266,7 +25262,7 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="110" t="s">
+      <c r="A146" s="109" t="s">
         <v>459</v>
       </c>
       <c r="B146" s="14" t="s">
@@ -25290,7 +25286,7 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="110" t="s">
+      <c r="A147" s="109" t="s">
         <v>460</v>
       </c>
       <c r="B147" s="14" t="n">
@@ -25314,7 +25310,7 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="110" t="s">
+      <c r="A148" s="109" t="s">
         <v>461</v>
       </c>
       <c r="B148" s="14" t="n">
@@ -25338,7 +25334,7 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="110" t="s">
+      <c r="A149" s="109" t="s">
         <v>462</v>
       </c>
       <c r="B149" s="14" t="n">
@@ -25362,7 +25358,7 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="110" t="s">
+      <c r="A150" s="109" t="s">
         <v>463</v>
       </c>
       <c r="B150" s="14" t="n">
@@ -25386,7 +25382,7 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="110" t="s">
+      <c r="A151" s="109" t="s">
         <v>464</v>
       </c>
       <c r="B151" s="14" t="str">
@@ -25411,7 +25407,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="110" t="s">
+      <c r="A152" s="109" t="s">
         <v>465</v>
       </c>
       <c r="B152" s="0"/>
@@ -25431,7 +25427,7 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="110" t="s">
+      <c r="A153" s="109" t="s">
         <v>466</v>
       </c>
       <c r="B153" s="0"/>
@@ -25451,7 +25447,7 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="110" t="s">
+      <c r="A154" s="109" t="s">
         <v>467</v>
       </c>
       <c r="B154" s="14" t="str">
@@ -25476,7 +25472,7 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="110" t="s">
+      <c r="A155" s="109" t="s">
         <v>470</v>
       </c>
       <c r="B155" s="14" t="str">
@@ -25504,7 +25500,7 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="110" t="s">
+      <c r="A156" s="109" t="s">
         <v>472</v>
       </c>
       <c r="B156" s="14" t="str">
@@ -25529,11 +25525,11 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="110" t="s">
+      <c r="A157" s="109" t="s">
         <v>473</v>
       </c>
       <c r="B157" s="5"/>
-      <c r="C157" s="110" t="s">
+      <c r="C157" s="109" t="s">
         <v>474</v>
       </c>
       <c r="D157" s="0" t="n">
@@ -25553,7 +25549,7 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="110" t="s">
+      <c r="A158" s="109" t="s">
         <v>476</v>
       </c>
       <c r="B158" s="14" t="str">
@@ -25581,7 +25577,7 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="110" t="s">
+      <c r="A159" s="109" t="s">
         <v>478</v>
       </c>
       <c r="B159" s="14" t="str">
@@ -25609,7 +25605,7 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="110" t="s">
+      <c r="A160" s="109" t="s">
         <v>479</v>
       </c>
       <c r="B160" s="14" t="str">
@@ -25634,7 +25630,7 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="110" t="s">
+      <c r="A161" s="109" t="s">
         <v>480</v>
       </c>
       <c r="B161" s="14" t="str">
@@ -25662,7 +25658,7 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="110" t="s">
+      <c r="A162" s="109" t="s">
         <v>482</v>
       </c>
       <c r="B162" s="14" t="str">
@@ -25687,7 +25683,7 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="110" t="s">
+      <c r="A163" s="109" t="s">
         <v>483</v>
       </c>
       <c r="B163" s="14" t="str">
@@ -25715,7 +25711,7 @@
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="110" t="s">
+      <c r="A164" s="109" t="s">
         <v>485</v>
       </c>
       <c r="B164" s="14" t="str">
@@ -25743,7 +25739,7 @@
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="110" t="s">
+      <c r="A165" s="109" t="s">
         <v>486</v>
       </c>
       <c r="B165" s="14" t="s">
@@ -25769,7 +25765,7 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="110" t="s">
+      <c r="A166" s="109" t="s">
         <v>489</v>
       </c>
       <c r="B166" s="14" t="s">
@@ -25796,7 +25792,7 @@
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="110" t="s">
+      <c r="A167" s="109" t="s">
         <v>492</v>
       </c>
       <c r="B167" s="14" t="s">
@@ -25820,7 +25816,7 @@
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="110" t="s">
+      <c r="A168" s="109" t="s">
         <v>494</v>
       </c>
       <c r="B168" s="14" t="s">
@@ -25847,7 +25843,7 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="110" t="s">
+      <c r="A169" s="109" t="s">
         <v>496</v>
       </c>
       <c r="B169" s="14" t="str">
@@ -25875,7 +25871,7 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="110" t="s">
+      <c r="A170" s="109" t="s">
         <v>498</v>
       </c>
       <c r="B170" s="14" t="str">
@@ -25903,7 +25899,7 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="110" t="s">
+      <c r="A171" s="109" t="s">
         <v>500</v>
       </c>
       <c r="B171" s="14" t="str">
@@ -25928,7 +25924,7 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="110" t="s">
+      <c r="A172" s="109" t="s">
         <v>503</v>
       </c>
       <c r="B172" s="14" t="str">
@@ -25956,7 +25952,7 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="110" t="s">
+      <c r="A173" s="109" t="s">
         <v>504</v>
       </c>
       <c r="B173" s="14" t="str">
@@ -25981,7 +25977,7 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="110" t="s">
+      <c r="A174" s="109" t="s">
         <v>505</v>
       </c>
       <c r="B174" s="14" t="str">
@@ -26006,7 +26002,7 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="110" t="s">
+      <c r="A175" s="109" t="s">
         <v>506</v>
       </c>
       <c r="B175" s="14" t="str">
@@ -26031,7 +26027,7 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="110" t="s">
+      <c r="A176" s="109" t="s">
         <v>507</v>
       </c>
       <c r="B176" s="14" t="str">
@@ -26059,7 +26055,7 @@
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="110" t="s">
+      <c r="A177" s="109" t="s">
         <v>508</v>
       </c>
       <c r="B177" s="14" t="str">
@@ -26087,7 +26083,7 @@
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="110" t="s">
+      <c r="A178" s="109" t="s">
         <v>509</v>
       </c>
       <c r="B178" s="14" t="str">
@@ -26117,7 +26113,7 @@
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="110" t="s">
+      <c r="A179" s="109" t="s">
         <v>511</v>
       </c>
       <c r="B179" s="14" t="str">
@@ -26142,7 +26138,7 @@
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="110" t="s">
+      <c r="A180" s="109" t="s">
         <v>512</v>
       </c>
       <c r="B180" s="14" t="str">
@@ -26167,7 +26163,7 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="110" t="s">
+      <c r="A181" s="109" t="s">
         <v>513</v>
       </c>
       <c r="B181" s="14" t="str">
@@ -26192,7 +26188,7 @@
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="110" t="s">
+      <c r="A182" s="109" t="s">
         <v>514</v>
       </c>
       <c r="B182" s="14" t="str">
@@ -26217,7 +26213,7 @@
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="110" t="s">
+      <c r="A183" s="109" t="s">
         <v>515</v>
       </c>
       <c r="B183" s="14" t="str">
@@ -26242,7 +26238,7 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="110" t="s">
+      <c r="A184" s="109" t="s">
         <v>516</v>
       </c>
       <c r="B184" s="14" t="str">
@@ -26267,7 +26263,7 @@
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="110" t="s">
+      <c r="A185" s="109" t="s">
         <v>517</v>
       </c>
       <c r="B185" s="14" t="str">
@@ -26292,7 +26288,7 @@
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="110" t="s">
+      <c r="A186" s="109" t="s">
         <v>518</v>
       </c>
       <c r="B186" s="14" t="n">
@@ -26316,7 +26312,7 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="110" t="s">
+      <c r="A187" s="109" t="s">
         <v>520</v>
       </c>
       <c r="B187" s="14" t="n">
@@ -26340,7 +26336,7 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="110" t="s">
+      <c r="A188" s="109" t="s">
         <v>522</v>
       </c>
       <c r="B188" s="14" t="str">
@@ -26365,7 +26361,7 @@
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="110" t="s">
+      <c r="A189" s="109" t="s">
         <v>523</v>
       </c>
       <c r="B189" s="14" t="str">
@@ -26390,7 +26386,7 @@
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="110" t="s">
+      <c r="A190" s="109" t="s">
         <v>524</v>
       </c>
       <c r="B190" s="14" t="str">
@@ -26415,7 +26411,7 @@
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="110" t="s">
+      <c r="A191" s="109" t="s">
         <v>525</v>
       </c>
       <c r="B191" s="14" t="str">
@@ -26438,12 +26434,12 @@
       <c r="H191" s="14" t="s">
         <v>502</v>
       </c>
-      <c r="J191" s="111" t="s">
+      <c r="J191" s="110" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="110" t="s">
+      <c r="A192" s="109" t="s">
         <v>527</v>
       </c>
       <c r="B192" s="14" t="str">
@@ -26468,7 +26464,7 @@
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="110" t="s">
+      <c r="A193" s="109" t="s">
         <v>528</v>
       </c>
       <c r="B193" s="14" t="str">
@@ -26493,7 +26489,7 @@
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="110" t="s">
+      <c r="A194" s="109" t="s">
         <v>529</v>
       </c>
       <c r="B194" s="14" t="str">
@@ -26518,7 +26514,7 @@
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="110" t="s">
+      <c r="A195" s="109" t="s">
         <v>530</v>
       </c>
       <c r="B195" s="14" t="str">
@@ -26543,7 +26539,7 @@
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="110" t="s">
+      <c r="A196" s="109" t="s">
         <v>532</v>
       </c>
       <c r="B196" s="14" t="str">
@@ -26568,7 +26564,7 @@
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="110" t="s">
+      <c r="A197" s="109" t="s">
         <v>533</v>
       </c>
       <c r="B197" s="14" t="str">
@@ -26593,7 +26589,7 @@
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="110" t="s">
+      <c r="A198" s="109" t="s">
         <v>534</v>
       </c>
       <c r="B198" s="14" t="str">
@@ -26618,7 +26614,7 @@
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="110" t="s">
+      <c r="A199" s="109" t="s">
         <v>535</v>
       </c>
       <c r="B199" s="14" t="str">
@@ -26643,7 +26639,7 @@
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="110" t="s">
+      <c r="A200" s="109" t="s">
         <v>536</v>
       </c>
       <c r="B200" s="14" t="n">
@@ -26667,7 +26663,7 @@
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="110" t="s">
+      <c r="A201" s="109" t="s">
         <v>540</v>
       </c>
       <c r="B201" s="14" t="n">
@@ -26691,7 +26687,7 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="110" t="s">
+      <c r="A202" s="109" t="s">
         <v>542</v>
       </c>
       <c r="B202" s="14" t="n">
@@ -26715,7 +26711,7 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="110" t="s">
+      <c r="A203" s="109" t="s">
         <v>544</v>
       </c>
       <c r="B203" s="14" t="n">
@@ -26739,7 +26735,7 @@
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="110" t="s">
+      <c r="A204" s="109" t="s">
         <v>546</v>
       </c>
       <c r="B204" s="14" t="s">
@@ -26763,7 +26759,7 @@
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="110" t="s">
+      <c r="A205" s="109" t="s">
         <v>548</v>
       </c>
       <c r="B205" s="14" t="n">
@@ -26787,7 +26783,7 @@
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="110" t="s">
+      <c r="A206" s="109" t="s">
         <v>549</v>
       </c>
       <c r="B206" s="14" t="n">
@@ -26811,7 +26807,7 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="110" t="s">
+      <c r="A207" s="109" t="s">
         <v>550</v>
       </c>
       <c r="B207" s="14" t="s">
@@ -26835,7 +26831,7 @@
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="110" t="s">
+      <c r="A208" s="109" t="s">
         <v>551</v>
       </c>
       <c r="B208" s="14" t="s">
@@ -26859,7 +26855,7 @@
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="110" t="s">
+      <c r="A209" s="109" t="s">
         <v>552</v>
       </c>
       <c r="B209" s="14" t="s">
@@ -26883,7 +26879,7 @@
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="110" t="s">
+      <c r="A210" s="109" t="s">
         <v>553</v>
       </c>
       <c r="B210" s="14" t="s">
@@ -26912,7 +26908,7 @@
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="110" t="s">
+      <c r="A211" s="109" t="s">
         <v>556</v>
       </c>
       <c r="B211" s="14" t="n">
@@ -26936,7 +26932,7 @@
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="110" t="s">
+      <c r="A212" s="109" t="s">
         <v>558</v>
       </c>
       <c r="B212" s="14" t="n">
@@ -26960,7 +26956,7 @@
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="110" t="s">
+      <c r="A213" s="109" t="s">
         <v>559</v>
       </c>
       <c r="B213" s="14" t="n">
@@ -26984,7 +26980,7 @@
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="110" t="s">
+      <c r="A214" s="109" t="s">
         <v>560</v>
       </c>
       <c r="B214" s="14" t="n">
@@ -27008,7 +27004,7 @@
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="110" t="s">
+      <c r="A215" s="109" t="s">
         <v>561</v>
       </c>
       <c r="B215" s="14" t="n">
@@ -27032,7 +27028,7 @@
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="110" t="s">
+      <c r="A216" s="109" t="s">
         <v>370</v>
       </c>
       <c r="B216" s="0"/>
@@ -27050,7 +27046,7 @@
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="110" t="s">
+      <c r="A217" s="109" t="s">
         <v>562</v>
       </c>
       <c r="B217" s="14" t="n">
@@ -27074,7 +27070,7 @@
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="110" t="s">
+      <c r="A218" s="109" t="s">
         <v>564</v>
       </c>
       <c r="B218" s="14" t="n">
@@ -27098,7 +27094,7 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="110" t="s">
+      <c r="A219" s="109" t="s">
         <v>565</v>
       </c>
       <c r="B219" s="14" t="n">
@@ -27122,7 +27118,7 @@
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="110" t="s">
+      <c r="A220" s="109" t="s">
         <v>566</v>
       </c>
       <c r="B220" s="14" t="n">
@@ -27146,7 +27142,7 @@
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="110" t="s">
+      <c r="A221" s="109" t="s">
         <v>567</v>
       </c>
       <c r="B221" s="14" t="s">
@@ -27170,7 +27166,7 @@
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="110" t="s">
+      <c r="A222" s="109" t="s">
         <v>568</v>
       </c>
       <c r="B222" s="14" t="n">
@@ -27194,7 +27190,7 @@
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="110" t="s">
+      <c r="A223" s="109" t="s">
         <v>569</v>
       </c>
       <c r="B223" s="14" t="s">
@@ -27218,7 +27214,7 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="110" t="s">
+      <c r="A224" s="109" t="s">
         <v>570</v>
       </c>
       <c r="B224" s="14" t="s">
@@ -27242,7 +27238,7 @@
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="110" t="s">
+      <c r="A225" s="109" t="s">
         <v>571</v>
       </c>
       <c r="B225" s="14" t="s">
@@ -27268,7 +27264,7 @@
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="110" t="s">
+      <c r="A226" s="109" t="s">
         <v>572</v>
       </c>
       <c r="B226" s="14" t="n">
@@ -27292,7 +27288,7 @@
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="110" t="s">
+      <c r="A227" s="109" t="s">
         <v>573</v>
       </c>
       <c r="B227" s="14" t="n">
@@ -27316,7 +27312,7 @@
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="110" t="s">
+      <c r="A228" s="109" t="s">
         <v>574</v>
       </c>
       <c r="B228" s="14" t="n">
@@ -27340,7 +27336,7 @@
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="110" t="s">
+      <c r="A229" s="109" t="s">
         <v>575</v>
       </c>
       <c r="B229" s="14" t="n">
@@ -27364,7 +27360,7 @@
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="110" t="s">
+      <c r="A230" s="109" t="s">
         <v>576</v>
       </c>
       <c r="B230" s="14" t="n">
@@ -28563,7 +28559,7 @@
       <c r="A279" s="14" t="s">
         <v>647</v>
       </c>
-      <c r="B279" s="112" t="s">
+      <c r="B279" s="111" t="s">
         <v>190</v>
       </c>
       <c r="C279" s="5" t="s">
@@ -28589,7 +28585,7 @@
       <c r="A280" s="14" t="s">
         <v>648</v>
       </c>
-      <c r="B280" s="112" t="s">
+      <c r="B280" s="111" t="s">
         <v>190</v>
       </c>
       <c r="C280" s="5" t="s">
@@ -28615,7 +28611,7 @@
       <c r="A281" s="14" t="s">
         <v>649</v>
       </c>
-      <c r="B281" s="112" t="s">
+      <c r="B281" s="111" t="s">
         <v>190</v>
       </c>
       <c r="C281" s="5" t="s">
@@ -28641,7 +28637,7 @@
       <c r="A282" s="14" t="s">
         <v>651</v>
       </c>
-      <c r="B282" s="112" t="s">
+      <c r="B282" s="111" t="s">
         <v>190</v>
       </c>
       <c r="C282" s="5" t="s">
@@ -28844,8 +28840,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -28880,7 +28876,7 @@
       <c r="A2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="112" t="s">
         <v>666</v>
       </c>
     </row>
@@ -28888,7 +28884,7 @@
       <c r="A3" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="112" t="s">
         <v>667</v>
       </c>
     </row>
@@ -28896,7 +28892,7 @@
       <c r="A4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="113" t="s">
+      <c r="B4" s="112" t="s">
         <v>668</v>
       </c>
     </row>
@@ -28904,7 +28900,7 @@
       <c r="A5" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="113" t="s">
+      <c r="B5" s="112" t="s">
         <v>669</v>
       </c>
     </row>
@@ -28912,7 +28908,7 @@
       <c r="A6" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="113" t="s">
+      <c r="B6" s="112" t="s">
         <v>670</v>
       </c>
     </row>
@@ -28920,7 +28916,7 @@
       <c r="A7" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="113" t="s">
+      <c r="B7" s="112" t="s">
         <v>671</v>
       </c>
     </row>
@@ -28928,7 +28924,7 @@
       <c r="A8" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="113" t="s">
+      <c r="B8" s="112" t="s">
         <v>672</v>
       </c>
     </row>
@@ -28936,7 +28932,7 @@
       <c r="A9" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="113" t="s">
+      <c r="B9" s="112" t="s">
         <v>673</v>
       </c>
     </row>
@@ -28944,7 +28940,7 @@
       <c r="A10" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="113" t="s">
+      <c r="B10" s="112" t="s">
         <v>674</v>
       </c>
     </row>
@@ -28952,7 +28948,7 @@
       <c r="A11" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="113" t="s">
+      <c r="B11" s="112" t="s">
         <v>675</v>
       </c>
     </row>
@@ -28960,7 +28956,7 @@
       <c r="A12" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="113" t="s">
+      <c r="B12" s="112" t="s">
         <v>676</v>
       </c>
     </row>
@@ -28968,7 +28964,7 @@
       <c r="A13" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="112" t="s">
         <v>677</v>
       </c>
     </row>
@@ -28976,7 +28972,7 @@
       <c r="A14" s="2" t="n">
         <v>25304</v>
       </c>
-      <c r="B14" s="113" t="s">
+      <c r="B14" s="112" t="s">
         <v>678</v>
       </c>
     </row>
@@ -28996,7 +28992,7 @@
       <c r="A17" s="2" t="n">
         <v>33460</v>
       </c>
-      <c r="B17" s="113" t="s">
+      <c r="B17" s="112" t="s">
         <v>679</v>
       </c>
     </row>
@@ -29004,7 +29000,7 @@
       <c r="A18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="113" t="s">
+      <c r="B18" s="112" t="s">
         <v>667</v>
       </c>
     </row>
@@ -29012,7 +29008,7 @@
       <c r="A19" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B19" s="113" t="s">
+      <c r="B19" s="112" t="s">
         <v>680</v>
       </c>
     </row>
@@ -29020,7 +29016,7 @@
       <c r="A20" s="2" t="n">
         <v>18601</v>
       </c>
-      <c r="B20" s="113" t="s">
+      <c r="B20" s="112" t="s">
         <v>681</v>
       </c>
     </row>
@@ -29028,7 +29024,7 @@
       <c r="A21" s="2" t="n">
         <v>20979</v>
       </c>
-      <c r="B21" s="113" t="s">
+      <c r="B21" s="112" t="s">
         <v>678</v>
       </c>
     </row>
@@ -29036,7 +29032,7 @@
       <c r="A22" s="2" t="n">
         <v>23030</v>
       </c>
-      <c r="B22" s="113" t="s">
+      <c r="B22" s="112" t="s">
         <v>682</v>
       </c>
     </row>
@@ -29050,7 +29046,7 @@
       <c r="A24" s="2" t="n">
         <v>27548</v>
       </c>
-      <c r="B24" s="113" t="s">
+      <c r="B24" s="112" t="s">
         <v>683</v>
       </c>
     </row>
@@ -29058,7 +29054,7 @@
       <c r="A25" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B25" s="113" t="s">
+      <c r="B25" s="112" t="s">
         <v>684</v>
       </c>
     </row>
@@ -29066,7 +29062,7 @@
       <c r="A26" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B26" s="113" t="s">
+      <c r="B26" s="112" t="s">
         <v>672</v>
       </c>
     </row>
@@ -29074,7 +29070,7 @@
       <c r="A27" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B27" s="113" t="s">
+      <c r="B27" s="112" t="s">
         <v>673</v>
       </c>
     </row>
@@ -29082,7 +29078,7 @@
       <c r="A28" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="113" t="s">
+      <c r="B28" s="112" t="s">
         <v>674</v>
       </c>
     </row>
@@ -29090,7 +29086,7 @@
       <c r="A29" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="113" t="s">
+      <c r="B29" s="112" t="s">
         <v>676</v>
       </c>
     </row>
@@ -29098,7 +29094,7 @@
       <c r="A30" s="2" t="n">
         <v>20883</v>
       </c>
-      <c r="B30" s="113" t="s">
+      <c r="B30" s="112" t="s">
         <v>681</v>
       </c>
     </row>
@@ -29112,7 +29108,7 @@
       <c r="A32" s="2" t="n">
         <v>27993</v>
       </c>
-      <c r="B32" s="113" t="s">
+      <c r="B32" s="112" t="s">
         <v>683</v>
       </c>
     </row>
@@ -29120,7 +29116,7 @@
       <c r="A33" s="2" t="n">
         <v>31023</v>
       </c>
-      <c r="B33" s="113" t="s">
+      <c r="B33" s="112" t="s">
         <v>679</v>
       </c>
     </row>
@@ -29128,7 +29124,7 @@
       <c r="A34" s="2" t="n">
         <v>33873</v>
       </c>
-      <c r="B34" s="113" t="s">
+      <c r="B34" s="112" t="s">
         <v>682</v>
       </c>
     </row>
@@ -29136,7 +29132,7 @@
       <c r="A35" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B35" s="113" t="s">
+      <c r="B35" s="112" t="s">
         <v>676</v>
       </c>
     </row>
@@ -29144,7 +29140,7 @@
       <c r="A36" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B36" s="113" t="s">
+      <c r="B36" s="112" t="s">
         <v>685</v>
       </c>
     </row>
@@ -29152,7 +29148,7 @@
       <c r="A37" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="113" t="s">
+      <c r="B37" s="112" t="s">
         <v>672</v>
       </c>
     </row>
@@ -29160,7 +29156,7 @@
       <c r="A38" s="2" t="n">
         <v>26585</v>
       </c>
-      <c r="B38" s="113" t="s">
+      <c r="B38" s="112" t="s">
         <v>678</v>
       </c>
     </row>
@@ -29168,7 +29164,7 @@
       <c r="A39" s="2" t="n">
         <v>27717</v>
       </c>
-      <c r="B39" s="113" t="s">
+      <c r="B39" s="112" t="s">
         <v>682</v>
       </c>
     </row>
@@ -29182,7 +29178,7 @@
       <c r="A41" s="2" t="n">
         <v>33089</v>
       </c>
-      <c r="B41" s="113" t="s">
+      <c r="B41" s="112" t="s">
         <v>683</v>
       </c>
     </row>
@@ -29190,7 +29186,7 @@
       <c r="A42" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B42" s="113" t="s">
+      <c r="B42" s="112" t="s">
         <v>686</v>
       </c>
     </row>
@@ -29198,7 +29194,7 @@
       <c r="A43" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="113" t="s">
+      <c r="B43" s="112" t="s">
         <v>685</v>
       </c>
     </row>
@@ -29206,7 +29202,7 @@
       <c r="A44" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="113" t="s">
+      <c r="B44" s="112" t="s">
         <v>675</v>
       </c>
     </row>
@@ -29214,7 +29210,7 @@
       <c r="A45" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="113" t="s">
+      <c r="B45" s="112" t="s">
         <v>667</v>
       </c>
     </row>
@@ -29222,7 +29218,7 @@
       <c r="A46" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B46" s="113" t="s">
+      <c r="B46" s="112" t="s">
         <v>674</v>
       </c>
     </row>
@@ -29230,7 +29226,7 @@
       <c r="A47" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B47" s="113" t="s">
+      <c r="B47" s="112" t="s">
         <v>687</v>
       </c>
     </row>
@@ -29238,7 +29234,7 @@
       <c r="A48" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="113" t="s">
+      <c r="B48" s="112" t="s">
         <v>684</v>
       </c>
     </row>
@@ -29246,7 +29242,7 @@
       <c r="A49" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B49" s="113" t="s">
+      <c r="B49" s="112" t="s">
         <v>671</v>
       </c>
     </row>
@@ -29254,7 +29250,7 @@
       <c r="A50" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B50" s="113" t="s">
+      <c r="B50" s="112" t="s">
         <v>685</v>
       </c>
     </row>
@@ -29262,7 +29258,7 @@
       <c r="A51" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B51" s="113" t="s">
+      <c r="B51" s="112" t="s">
         <v>675</v>
       </c>
     </row>
@@ -29270,7 +29266,7 @@
       <c r="A52" s="2" t="n">
         <v>3640</v>
       </c>
-      <c r="B52" s="113" t="s">
+      <c r="B52" s="112" t="s">
         <v>682</v>
       </c>
     </row>
@@ -29278,7 +29274,7 @@
       <c r="A53" s="2" t="n">
         <v>4698</v>
       </c>
-      <c r="B53" s="113" t="s">
+      <c r="B53" s="112" t="s">
         <v>679</v>
       </c>
     </row>
@@ -29298,7 +29294,7 @@
       <c r="A56" s="2" t="n">
         <v>10264</v>
       </c>
-      <c r="B56" s="113" t="s">
+      <c r="B56" s="112" t="s">
         <v>669</v>
       </c>
     </row>
@@ -29306,7 +29302,7 @@
       <c r="A57" s="2" t="n">
         <v>10756</v>
       </c>
-      <c r="B57" s="113" t="s">
+      <c r="B57" s="112" t="s">
         <v>688</v>
       </c>
     </row>
@@ -29314,7 +29310,7 @@
       <c r="A58" s="2" t="n">
         <v>12879</v>
       </c>
-      <c r="B58" s="113" t="s">
+      <c r="B58" s="112" t="s">
         <v>677</v>
       </c>
     </row>
@@ -29322,7 +29318,7 @@
       <c r="A59" s="2" t="n">
         <v>14908</v>
       </c>
-      <c r="B59" s="113" t="s">
+      <c r="B59" s="112" t="s">
         <v>689</v>
       </c>
     </row>
@@ -29330,7 +29326,7 @@
       <c r="A60" s="2" t="n">
         <v>18140</v>
       </c>
-      <c r="B60" s="113" t="s">
+      <c r="B60" s="112" t="s">
         <v>666</v>
       </c>
     </row>
@@ -29338,7 +29334,7 @@
       <c r="A61" s="2" t="n">
         <v>21484</v>
       </c>
-      <c r="B61" s="113" t="s">
+      <c r="B61" s="112" t="s">
         <v>686</v>
       </c>
     </row>
@@ -29346,7 +29342,7 @@
       <c r="A62" s="2" t="n">
         <v>24890</v>
       </c>
-      <c r="B62" s="113" t="s">
+      <c r="B62" s="112" t="s">
         <v>680</v>
       </c>
     </row>
@@ -29354,7 +29350,7 @@
       <c r="A63" s="2" t="n">
         <v>28929</v>
       </c>
-      <c r="B63" s="113" t="s">
+      <c r="B63" s="112" t="s">
         <v>673</v>
       </c>
     </row>
@@ -29362,7 +29358,7 @@
       <c r="A64" s="2" t="n">
         <v>31440</v>
       </c>
-      <c r="B64" s="113" t="s">
+      <c r="B64" s="112" t="s">
         <v>690</v>
       </c>
     </row>
@@ -29370,7 +29366,7 @@
       <c r="A65" s="2" t="n">
         <v>34493</v>
       </c>
-      <c r="B65" s="113" t="s">
+      <c r="B65" s="112" t="s">
         <v>691</v>
       </c>
     </row>
@@ -29378,7 +29374,7 @@
       <c r="A66" s="2" t="n">
         <v>14799</v>
       </c>
-      <c r="B66" s="113" t="s">
+      <c r="B66" s="112" t="s">
         <v>666</v>
       </c>
     </row>
@@ -29386,7 +29382,7 @@
       <c r="A67" s="2" t="n">
         <v>15611</v>
       </c>
-      <c r="B67" s="113" t="s">
+      <c r="B67" s="112" t="s">
         <v>669</v>
       </c>
     </row>
@@ -29394,7 +29390,7 @@
       <c r="A68" s="2" t="n">
         <v>18113</v>
       </c>
-      <c r="B68" s="113" t="s">
+      <c r="B68" s="112" t="s">
         <v>677</v>
       </c>
     </row>
@@ -29402,7 +29398,7 @@
       <c r="A69" s="2" t="n">
         <v>21006</v>
       </c>
-      <c r="B69" s="113" t="s">
+      <c r="B69" s="112" t="s">
         <v>680</v>
       </c>
     </row>
@@ -29410,7 +29406,7 @@
       <c r="A70" s="2" t="n">
         <v>23919</v>
       </c>
-      <c r="B70" s="113" t="s">
+      <c r="B70" s="112" t="s">
         <v>689</v>
       </c>
     </row>
@@ -29418,7 +29414,7 @@
       <c r="A71" s="2" t="n">
         <v>26477</v>
       </c>
-      <c r="B71" s="113" t="s">
+      <c r="B71" s="112" t="s">
         <v>686</v>
       </c>
     </row>
@@ -29426,7 +29422,7 @@
       <c r="A72" s="2" t="n">
         <v>29184</v>
       </c>
-      <c r="B72" s="113" t="s">
+      <c r="B72" s="112" t="s">
         <v>691</v>
       </c>
     </row>
@@ -29440,7 +29436,7 @@
       <c r="A74" s="2" t="n">
         <v>11686</v>
       </c>
-      <c r="B74" s="113" t="s">
+      <c r="B74" s="112" t="s">
         <v>670</v>
       </c>
     </row>
@@ -29448,7 +29444,7 @@
       <c r="A75" s="2" t="n">
         <v>12402</v>
       </c>
-      <c r="B75" s="113" t="s">
+      <c r="B75" s="112" t="s">
         <v>687</v>
       </c>
     </row>
@@ -29456,7 +29452,7 @@
       <c r="A76" s="2" t="n">
         <v>16311</v>
       </c>
-      <c r="B76" s="113" t="s">
+      <c r="B76" s="112" t="s">
         <v>666</v>
       </c>
     </row>
@@ -29464,7 +29460,7 @@
       <c r="A77" s="2" t="n">
         <v>18798</v>
       </c>
-      <c r="B77" s="113" t="s">
+      <c r="B77" s="112" t="s">
         <v>689</v>
       </c>
     </row>
@@ -29472,7 +29468,7 @@
       <c r="A78" s="2" t="n">
         <v>23058</v>
       </c>
-      <c r="B78" s="113" t="s">
+      <c r="B78" s="112" t="s">
         <v>668</v>
       </c>
     </row>
@@ -29480,7 +29476,7 @@
       <c r="A79" s="2" t="n">
         <v>25775</v>
       </c>
-      <c r="B79" s="113" t="s">
+      <c r="B79" s="112" t="s">
         <v>684</v>
       </c>
     </row>
@@ -29488,7 +29484,7 @@
       <c r="A80" s="2" t="n">
         <v>28338</v>
       </c>
-      <c r="B80" s="113" t="s">
+      <c r="B80" s="112" t="s">
         <v>692</v>
       </c>
     </row>
@@ -29496,7 +29492,7 @@
       <c r="A81" s="2" t="n">
         <v>30847</v>
       </c>
-      <c r="B81" s="113" t="s">
+      <c r="B81" s="112" t="s">
         <v>691</v>
       </c>
     </row>
@@ -29504,7 +29500,7 @@
       <c r="A82" s="2" t="n">
         <v>3174</v>
       </c>
-      <c r="B82" s="113" t="s">
+      <c r="B82" s="112" t="s">
         <v>668</v>
       </c>
     </row>
@@ -29512,7 +29508,7 @@
       <c r="A83" s="2" t="n">
         <v>3199</v>
       </c>
-      <c r="B83" s="113" t="s">
+      <c r="B83" s="112" t="s">
         <v>690</v>
       </c>
     </row>
@@ -29520,7 +29516,7 @@
       <c r="A84" s="2" t="n">
         <v>3265</v>
       </c>
-      <c r="B84" s="113" t="s">
+      <c r="B84" s="112" t="s">
         <v>692</v>
       </c>
     </row>
@@ -29528,7 +29524,7 @@
       <c r="A85" s="2" t="n">
         <v>3722</v>
       </c>
-      <c r="B85" s="113" t="s">
+      <c r="B85" s="112" t="s">
         <v>678</v>
       </c>
     </row>
@@ -29536,7 +29532,7 @@
       <c r="A86" s="2" t="n">
         <v>3968</v>
       </c>
-      <c r="B86" s="113" t="s">
+      <c r="B86" s="112" t="s">
         <v>681</v>
       </c>
     </row>
@@ -29544,7 +29540,7 @@
       <c r="A87" s="2" t="n">
         <v>4955</v>
       </c>
-      <c r="B87" s="113" t="s">
+      <c r="B87" s="112" t="s">
         <v>666</v>
       </c>
     </row>
@@ -29552,7 +29548,7 @@
       <c r="A88" s="2" t="n">
         <v>5862</v>
       </c>
-      <c r="B88" s="113" t="s">
+      <c r="B88" s="112" t="s">
         <v>688</v>
       </c>
     </row>
@@ -29560,7 +29556,7 @@
       <c r="A89" s="2" t="n">
         <v>6154</v>
       </c>
-      <c r="B89" s="113" t="s">
+      <c r="B89" s="112" t="s">
         <v>689</v>
       </c>
     </row>
@@ -29568,7 +29564,7 @@
       <c r="A90" s="2" t="n">
         <v>7686</v>
       </c>
-      <c r="B90" s="113" t="s">
+      <c r="B90" s="112" t="s">
         <v>671</v>
       </c>
     </row>
@@ -29576,7 +29572,7 @@
       <c r="A91" s="2" t="n">
         <v>7848</v>
       </c>
-      <c r="B91" s="113" t="s">
+      <c r="B91" s="112" t="s">
         <v>679</v>
       </c>
     </row>
@@ -29584,7 +29580,7 @@
       <c r="A92" s="2" t="n">
         <v>9985</v>
       </c>
-      <c r="B92" s="113" t="s">
+      <c r="B92" s="112" t="s">
         <v>683</v>
       </c>
     </row>
@@ -29628,7 +29624,7 @@
       <c r="A99" s="2" t="n">
         <v>21665</v>
       </c>
-      <c r="B99" s="113" t="s">
+      <c r="B99" s="112" t="s">
         <v>670</v>
       </c>
     </row>
@@ -29636,7 +29632,7 @@
       <c r="A100" s="2" t="n">
         <v>22499</v>
       </c>
-      <c r="B100" s="113" t="s">
+      <c r="B100" s="112" t="s">
         <v>688</v>
       </c>
     </row>
@@ -29644,7 +29640,7 @@
       <c r="A101" s="2" t="n">
         <v>24062</v>
       </c>
-      <c r="B101" s="113" t="s">
+      <c r="B101" s="112" t="s">
         <v>666</v>
       </c>
     </row>
@@ -29652,7 +29648,7 @@
       <c r="A102" s="2" t="n">
         <v>27134</v>
       </c>
-      <c r="B102" s="113" t="s">
+      <c r="B102" s="112" t="s">
         <v>687</v>
       </c>
     </row>
@@ -29660,7 +29656,7 @@
       <c r="A103" s="2" t="n">
         <v>29698</v>
       </c>
-      <c r="B103" s="113" t="s">
+      <c r="B103" s="112" t="s">
         <v>692</v>
       </c>
     </row>
@@ -29668,7 +29664,7 @@
       <c r="A104" s="2" t="n">
         <v>32311</v>
       </c>
-      <c r="B104" s="113" t="s">
+      <c r="B104" s="112" t="s">
         <v>690</v>
       </c>
     </row>
@@ -29676,7 +29672,7 @@
       <c r="A105" s="2" t="n">
         <v>34347</v>
       </c>
-      <c r="B105" s="113" t="s">
+      <c r="B105" s="112" t="s">
         <v>681</v>
       </c>
     </row>
@@ -29685,8 +29681,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -29747,7 +29743,7 @@
       <c r="A3" s="5" t="s">
         <v>698</v>
       </c>
-      <c r="B3" s="114" t="n">
+      <c r="B3" s="113" t="n">
         <v>41541</v>
       </c>
       <c r="C3" s="5" t="n">
@@ -29764,7 +29760,7 @@
       <c r="A4" s="5" t="s">
         <v>701</v>
       </c>
-      <c r="B4" s="114" t="n">
+      <c r="B4" s="113" t="n">
         <v>41626</v>
       </c>
       <c r="C4" s="5" t="n">
@@ -29781,7 +29777,7 @@
       <c r="A5" s="5" t="s">
         <v>703</v>
       </c>
-      <c r="B5" s="114" t="n">
+      <c r="B5" s="113" t="n">
         <v>41668</v>
       </c>
       <c r="C5" s="5" t="n">
@@ -29798,7 +29794,7 @@
       <c r="A6" s="5" t="s">
         <v>705</v>
       </c>
-      <c r="B6" s="114" t="n">
+      <c r="B6" s="113" t="n">
         <v>41680</v>
       </c>
       <c r="C6" s="5" t="n">
@@ -29815,7 +29811,7 @@
       <c r="A7" s="5" t="s">
         <v>708</v>
       </c>
-      <c r="B7" s="114" t="n">
+      <c r="B7" s="113" t="n">
         <v>41708</v>
       </c>
       <c r="C7" s="5" t="n">
@@ -29832,7 +29828,7 @@
       <c r="A8" s="5" t="s">
         <v>710</v>
       </c>
-      <c r="B8" s="114" t="n">
+      <c r="B8" s="113" t="n">
         <v>41731</v>
       </c>
       <c r="C8" s="5" t="n">
@@ -29849,7 +29845,7 @@
       <c r="A9" s="5" t="s">
         <v>712</v>
       </c>
-      <c r="B9" s="114" t="n">
+      <c r="B9" s="113" t="n">
         <v>41753</v>
       </c>
       <c r="C9" s="5" t="n">
@@ -29866,7 +29862,7 @@
       <c r="A10" s="5" t="s">
         <v>715</v>
       </c>
-      <c r="B10" s="114" t="n">
+      <c r="B10" s="113" t="n">
         <v>41792</v>
       </c>
       <c r="C10" s="5" t="n">
@@ -29883,7 +29879,7 @@
       <c r="A11" s="5" t="s">
         <v>717</v>
       </c>
-      <c r="B11" s="114" t="n">
+      <c r="B11" s="113" t="n">
         <v>41807</v>
       </c>
       <c r="C11" s="5" t="n">
@@ -29900,7 +29896,7 @@
       <c r="A12" s="5" t="s">
         <v>719</v>
       </c>
-      <c r="B12" s="114" t="n">
+      <c r="B12" s="113" t="n">
         <v>41876</v>
       </c>
       <c r="C12" s="5" t="n">
@@ -29917,7 +29913,7 @@
       <c r="A13" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="B13" s="115" t="n">
+      <c r="B13" s="114" t="n">
         <v>41887</v>
       </c>
       <c r="C13" s="5" t="n">
@@ -29932,7 +29928,7 @@
       <c r="A14" s="5" t="s">
         <v>723</v>
       </c>
-      <c r="B14" s="115" t="n">
+      <c r="B14" s="114" t="n">
         <v>41906</v>
       </c>
       <c r="C14" s="5" t="n">
@@ -29947,7 +29943,7 @@
       <c r="A15" s="5" t="s">
         <v>724</v>
       </c>
-      <c r="B15" s="115" t="n">
+      <c r="B15" s="114" t="n">
         <v>41926</v>
       </c>
       <c r="C15" s="5" t="n">
@@ -29971,8 +29967,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -29985,8 +29981,8 @@
   </sheetPr>
   <dimension ref="A1:H222"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -30032,7 +30028,7 @@
       <c r="A2" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="114" t="n">
+      <c r="B2" s="113" t="n">
         <v>41485</v>
       </c>
       <c r="C2" s="5" t="n">
@@ -30056,7 +30052,7 @@
       <c r="A3" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="B3" s="114" t="n">
+      <c r="B3" s="113" t="n">
         <v>41547</v>
       </c>
       <c r="C3" s="5" t="n">
@@ -30080,7 +30076,7 @@
       <c r="A4" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="B4" s="114" t="n">
+      <c r="B4" s="113" t="n">
         <v>41567</v>
       </c>
       <c r="C4" s="5" t="n">
@@ -30104,7 +30100,7 @@
       <c r="A5" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="B5" s="114" t="n">
+      <c r="B5" s="113" t="n">
         <v>41649</v>
       </c>
       <c r="C5" s="5" t="n">
@@ -30128,7 +30124,7 @@
       <c r="A6" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="B6" s="114" t="n">
+      <c r="B6" s="113" t="n">
         <v>41663</v>
       </c>
       <c r="C6" s="5" t="n">
@@ -30152,7 +30148,7 @@
       <c r="A7" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="B7" s="114" t="n">
+      <c r="B7" s="113" t="n">
         <v>41670</v>
       </c>
       <c r="C7" s="5" t="n">
@@ -30176,7 +30172,7 @@
       <c r="A8" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="B8" s="114" t="n">
+      <c r="B8" s="113" t="n">
         <v>41688</v>
       </c>
       <c r="C8" s="5" t="n">
@@ -30202,7 +30198,7 @@
       <c r="A9" s="5" t="s">
         <v>744</v>
       </c>
-      <c r="B9" s="114" t="n">
+      <c r="B9" s="113" t="n">
         <v>41710</v>
       </c>
       <c r="C9" s="5" t="n">
@@ -30226,7 +30222,7 @@
       <c r="A10" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="B10" s="114" t="n">
+      <c r="B10" s="113" t="n">
         <v>41716</v>
       </c>
       <c r="C10" s="5" t="n">
@@ -30252,7 +30248,7 @@
       <c r="A11" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="B11" s="114" t="n">
+      <c r="B11" s="113" t="n">
         <v>41738</v>
       </c>
       <c r="C11" s="5" t="n">
@@ -30276,7 +30272,7 @@
       <c r="A12" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="B12" s="114" t="n">
+      <c r="B12" s="113" t="n">
         <v>41759</v>
       </c>
       <c r="C12" s="5" t="n">
@@ -30300,7 +30296,7 @@
       <c r="A13" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="B13" s="114" t="n">
+      <c r="B13" s="113" t="n">
         <v>41771</v>
       </c>
       <c r="C13" s="5" t="n">
@@ -30324,7 +30320,7 @@
       <c r="A14" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="B14" s="114" t="n">
+      <c r="B14" s="113" t="n">
         <v>41779</v>
       </c>
       <c r="C14" s="5" t="n">
@@ -30350,7 +30346,7 @@
       <c r="A15" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="B15" s="114" t="n">
+      <c r="B15" s="113" t="n">
         <v>41784</v>
       </c>
       <c r="C15" s="5" t="n">
@@ -30376,7 +30372,7 @@
       <c r="A16" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="B16" s="114" t="n">
+      <c r="B16" s="113" t="n">
         <v>41801</v>
       </c>
       <c r="C16" s="5" t="n">
@@ -30402,7 +30398,7 @@
       <c r="A17" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="B17" s="114" t="n">
+      <c r="B17" s="113" t="n">
         <v>41807</v>
       </c>
       <c r="C17" s="5" t="n">
@@ -30428,7 +30424,7 @@
       <c r="A18" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="B18" s="114" t="n">
+      <c r="B18" s="113" t="n">
         <v>41829</v>
       </c>
       <c r="C18" s="5" t="n">
@@ -30454,7 +30450,7 @@
       <c r="A19" s="5" t="s">
         <v>501</v>
       </c>
-      <c r="B19" s="114" t="n">
+      <c r="B19" s="113" t="n">
         <v>41880</v>
       </c>
       <c r="C19" s="5" t="n">
@@ -30480,7 +30476,7 @@
       <c r="A20" s="5" t="s">
         <v>531</v>
       </c>
-      <c r="B20" s="114" t="n">
+      <c r="B20" s="113" t="n">
         <v>41887</v>
       </c>
       <c r="C20" s="5" t="n">
@@ -30506,7 +30502,7 @@
       <c r="A21" s="5" t="s">
         <v>537</v>
       </c>
-      <c r="B21" s="115" t="n">
+      <c r="B21" s="114" t="n">
         <v>41909</v>
       </c>
       <c r="C21" s="5" t="n">
@@ -30532,7 +30528,7 @@
       <c r="A22" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="B22" s="115" t="n">
+      <c r="B22" s="114" t="n">
         <v>41929</v>
       </c>
       <c r="C22" s="5" t="n">
@@ -30558,7 +30554,7 @@
       <c r="A23" s="5" t="s">
         <v>594</v>
       </c>
-      <c r="B23" s="115" t="n">
+      <c r="B23" s="114" t="n">
         <v>41943</v>
       </c>
       <c r="C23" s="5" t="n">
@@ -30584,7 +30580,7 @@
       <c r="A24" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="B24" s="115" t="n">
+      <c r="B24" s="114" t="n">
         <v>41963</v>
       </c>
       <c r="C24" s="5" t="n">
@@ -30610,7 +30606,7 @@
       <c r="A25" s="5" t="s">
         <v>640</v>
       </c>
-      <c r="B25" s="115" t="n">
+      <c r="B25" s="114" t="n">
         <v>41974</v>
       </c>
       <c r="C25" s="5" t="n">
@@ -30636,7 +30632,7 @@
       <c r="A26" s="5" t="s">
         <v>654</v>
       </c>
-      <c r="B26" s="115" t="n">
+      <c r="B26" s="114" t="n">
         <v>42037</v>
       </c>
       <c r="C26" s="5" t="n">
@@ -30669,8 +30665,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>